<commit_message>
No hay mucho más que se pueda hacer
</commit_message>
<xml_diff>
--- a/MicroSat/Iteraciones.xlsx
+++ b/MicroSat/Iteraciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\MEng Space Systems (Local)\2. EUE\Micro-Satellite Design &amp; Analysis\MicroSat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46C8C480-3555-4D1B-B557-9A9A8805FF03}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA06BFD3-B54A-4002-8BEE-EE4108B102BF}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>Nº rigidizadores</t>
   </si>
@@ -112,15 +112,22 @@
   </si>
   <si>
     <t>19x11mm</t>
+  </si>
+  <si>
+    <t>17x17mm</t>
+  </si>
+  <si>
+    <t>19x9.5mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -322,7 +329,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -414,12 +421,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="2" fillId="4" borderId="8" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,6 +453,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="8" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="7" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -738,10 +751,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -900,10 +913,10 @@
       <c r="G5" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="43">
+      <c r="H5" s="41">
         <v>57.86</v>
       </c>
-      <c r="I5" s="44">
+      <c r="I5" s="42">
         <f>H5-39.325-11</f>
         <v>7.5349999999999966</v>
       </c>
@@ -912,30 +925,30 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="39">
+      <c r="A6" s="37">
         <v>5</v>
       </c>
-      <c r="B6" s="40">
+      <c r="B6" s="38">
         <v>9</v>
       </c>
-      <c r="C6" s="41" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="41">
+      <c r="C6" s="39" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="39">
         <v>3</v>
       </c>
-      <c r="E6" s="41" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="41" t="s">
+      <c r="E6" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="41" t="s">
+      <c r="G6" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="41"/>
-      <c r="I6" s="41"/>
-      <c r="J6" s="42">
+      <c r="H6" s="39"/>
+      <c r="I6" s="39"/>
+      <c r="J6" s="40">
         <v>169.4</v>
       </c>
     </row>
@@ -1024,80 +1037,102 @@
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="36">
+      <c r="J9" s="34">
         <v>91.368440000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="29">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="8">
         <v>9</v>
       </c>
-      <c r="B10" s="30">
+      <c r="B10" s="28">
         <v>11</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
-      <c r="F10" s="31"/>
-      <c r="G10" s="31"/>
-      <c r="H10" s="31"/>
-      <c r="I10" s="31"/>
-      <c r="J10" s="32"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
-        <v>10</v>
-      </c>
-      <c r="B11" s="27">
-        <v>7</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="4">
+      <c r="C10" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="10">
+        <v>3</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="12">
+        <v>56.938980000000001</v>
+      </c>
+      <c r="I10" s="46">
+        <f>H10-39.325-11</f>
+        <v>6.613979999999998</v>
+      </c>
+      <c r="J10" s="34">
+        <v>90.916380000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="29">
+        <v>10</v>
+      </c>
+      <c r="B11" s="30">
+        <v>11</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="10">
+        <v>3</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="H11" s="44">
+        <v>58.935200000000002</v>
+      </c>
+      <c r="I11" s="45">
+        <f>H11-39.325-11</f>
+        <v>8.610199999999999</v>
+      </c>
+      <c r="J11" s="43">
+        <v>96.857420000000005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="27">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="4">
         <v>2</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H11" s="5"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="7">
+      <c r="H12" s="5"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7">
         <v>57.629820000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
-        <v>11</v>
-      </c>
-      <c r="B12" s="28">
-        <v>7</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="11">
-        <v>2</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="13"/>
-      <c r="J12" s="26">
-        <v>74.625</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.3">
@@ -1111,21 +1146,21 @@
         <v>7</v>
       </c>
       <c r="D13" s="11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="12"/>
+        <v>22</v>
+      </c>
+      <c r="H13" s="10"/>
       <c r="I13" s="13"/>
       <c r="J13" s="26">
-        <v>114.49639999999999</v>
+        <v>74.625</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
@@ -1145,18 +1180,16 @@
         <v>10</v>
       </c>
       <c r="F14" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G14" s="10" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H14" s="12"/>
       <c r="I14" s="13"/>
       <c r="J14" s="26">
-        <v>128.84270000000001</v>
-      </c>
-      <c r="K14" s="37"/>
-      <c r="L14" s="37"/>
+        <v>114.49639999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
@@ -1172,21 +1205,21 @@
         <v>3</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F15" s="10" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H15" s="12"/>
       <c r="I15" s="13"/>
-      <c r="J15" s="38">
-        <v>95.542420000000007</v>
-      </c>
-      <c r="K15" s="37"/>
-      <c r="L15" s="37"/>
+      <c r="J15" s="26">
+        <v>128.84270000000001</v>
+      </c>
+      <c r="K15" s="35"/>
+      <c r="L15" s="35"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
@@ -1198,56 +1231,86 @@
       <c r="C16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D16" s="10">
+      <c r="D16" s="11">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H16" s="12"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="36">
+        <v>95.542420000000007</v>
+      </c>
+      <c r="K16" s="35"/>
+      <c r="L16" s="35"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" s="8">
+        <v>16</v>
+      </c>
+      <c r="B17" s="28">
+        <v>7</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="10">
         <v>4</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="10" t="s">
+      <c r="E17" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G17" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="10"/>
-      <c r="I16" s="10"/>
-      <c r="J16" s="36">
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="34">
         <v>146.65029999999999</v>
       </c>
-      <c r="K16" s="37"/>
-      <c r="L16" s="37"/>
-    </row>
-    <row r="17" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="20">
+      <c r="K17" s="35"/>
+      <c r="L17" s="35"/>
+    </row>
+    <row r="18" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="20">
+        <v>17</v>
+      </c>
+      <c r="B18" s="21">
+        <v>7</v>
+      </c>
+      <c r="C18" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="22">
+        <v>4</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="21">
-        <v>7</v>
-      </c>
-      <c r="C17" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="22">
-        <v>4</v>
-      </c>
-      <c r="E17" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="22" t="s">
-        <v>16</v>
-      </c>
-      <c r="G17" s="22" t="s">
+      <c r="G18" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="34">
+      <c r="H18" s="32">
         <v>58.475189999999998</v>
       </c>
-      <c r="I17" s="35">
-        <f>H17-39.325-11</f>
+      <c r="I18" s="33">
+        <f>H18-39.325-11</f>
         <v>8.1501899999999949</v>
       </c>
-      <c r="J17" s="33">
+      <c r="J18" s="31">
         <v>154.22069999999999</v>
       </c>
     </row>
@@ -1259,17 +1322,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="c5ae091c-4d86-42b7-bd6d-05a6d5850206">
-      <UserInfo>
-        <DisplayName>Integrantes de la CURSO 1º MUSE</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1438,20 +1496,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="c5ae091c-4d86-42b7-bd6d-05a6d5850206">
+      <UserInfo>
+        <DisplayName>Integrantes de la CURSO 1º MUSE</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F2DDC3-8EF2-4F40-AEC5-CBD2E661EA55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A54CB81-BDC2-4F30-B8AA-8FF202FE488F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5ae091c-4d86-42b7-bd6d-05a6d5850206"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1476,9 +1537,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A54CB81-BDC2-4F30-B8AA-8FF202FE488F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F2DDC3-8EF2-4F40-AEC5-CBD2E661EA55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5ae091c-4d86-42b7-bd6d-05a6d5850206"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
27 ITERACIONES Y AÚN QUEDA
</commit_message>
<xml_diff>
--- a/MicroSat/Iteraciones.xlsx
+++ b/MicroSat/Iteraciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\MEng Space Systems (Local)\2. EUE\Micro-Satellite Design &amp; Analysis\MicroSat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE454C06-D220-4753-96CD-3E30E841048E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B865522C-A394-4093-872B-BB5F3D6B500B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="34">
   <si>
     <t>Nº rigidizadores</t>
   </si>
@@ -124,6 +124,18 @@
   </si>
   <si>
     <t>CBUSH (number)</t>
+  </si>
+  <si>
+    <t>RBE2 DOF</t>
+  </si>
+  <si>
+    <t>Posición RBE2 Mequip</t>
+  </si>
+  <si>
+    <t>Standard</t>
+  </si>
+  <si>
+    <t>Alejado</t>
   </si>
 </sst>
 </file>
@@ -343,14 +355,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -484,6 +493,36 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="5" borderId="5" xfId="4" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -769,770 +808,1157 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="10.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="2" max="2" width="11.77734375" customWidth="1"/>
     <col min="3" max="3" width="12.33203125" customWidth="1"/>
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="9" width="10.5546875" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.5546875" customWidth="1"/>
+    <col min="9" max="9" width="7.88671875" customWidth="1"/>
+    <col min="10" max="10" width="8.5546875" customWidth="1"/>
+    <col min="11" max="11" width="10.5546875" customWidth="1"/>
+    <col min="12" max="12" width="12" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="22" t="s">
+    <row r="1" spans="1:13" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="23" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="23" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="23" t="s">
+      <c r="D1" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="23" t="s">
+      <c r="F1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="23" t="s">
+      <c r="G1" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="I1" s="23" t="s">
+      <c r="I1" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="23" t="s">
+      <c r="L1" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="M1" s="23" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2" s="8">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3">
-        <v>8</v>
-      </c>
-      <c r="I2" s="5">
+      <c r="H2" s="9">
+        <v>8</v>
+      </c>
+      <c r="I2" s="9">
+        <v>123</v>
+      </c>
+      <c r="J2" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" s="11">
         <v>53.24</v>
       </c>
-      <c r="J2" s="6">
-        <f>I2-39.325-11</f>
+      <c r="L2" s="12">
+        <f>K2-39.325-11</f>
         <v>2.9149999999999991</v>
       </c>
-      <c r="K2" s="7">
+      <c r="M2" s="24">
         <v>64.605999999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="8">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" s="9">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="8">
         <v>9</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="11">
+      <c r="C3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="10">
+        <v>2</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="9">
+        <v>8</v>
+      </c>
+      <c r="I3" s="9">
+        <v>123456</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K3" s="11">
+        <v>53.24</v>
+      </c>
+      <c r="L3" s="12">
+        <f>K3-39.325-11</f>
+        <v>2.9149999999999991</v>
+      </c>
+      <c r="M3" s="24">
+        <v>83.861310000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="9">
         <v>3</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="G3" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="10">
-        <v>8</v>
-      </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="13"/>
-      <c r="K3" s="14">
-        <v>88.79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="8">
-        <v>3</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="B4" s="8">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="9" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="10">
         <v>3</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="10" t="s">
+      <c r="E4" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="9">
+        <v>8</v>
+      </c>
+      <c r="I4" s="9">
+        <v>123</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="13">
+        <v>88.79</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8">
+        <v>9</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5" s="9">
+        <v>3</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="10">
-        <v>8</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="15">
+      <c r="H5" s="9">
+        <v>8</v>
+      </c>
+      <c r="I5" s="9">
+        <v>123</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="14">
         <v>119.2757</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="16">
-        <v>4</v>
-      </c>
-      <c r="B5" s="48">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
+        <v>5</v>
+      </c>
+      <c r="B6" s="47">
         <v>9</v>
       </c>
-      <c r="C5" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="17">
+      <c r="C6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="16">
         <v>3</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" s="17" t="s">
+      <c r="E6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G6" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="17">
-        <v>8</v>
-      </c>
-      <c r="I5" s="39">
+      <c r="H6" s="16">
+        <v>8</v>
+      </c>
+      <c r="I6" s="16">
+        <v>123</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K6" s="38">
         <v>57.86</v>
       </c>
-      <c r="J5" s="40">
-        <f>I5-39.325-11</f>
+      <c r="L6" s="39">
+        <f>K6-39.325-11</f>
         <v>7.5349999999999966</v>
       </c>
-      <c r="K5" s="18">
+      <c r="M6" s="17">
         <v>152.38999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="16">
-        <v>5</v>
-      </c>
-      <c r="B6" s="48">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
+        <v>6</v>
+      </c>
+      <c r="B7" s="47">
         <v>9</v>
       </c>
-      <c r="C6" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="17">
+      <c r="C7" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7" s="16">
         <v>3</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="F6" s="17" t="s">
+      <c r="E7" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G7" s="16" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="17">
+      <c r="H7" s="16">
         <v>12</v>
       </c>
-      <c r="I6" s="39">
+      <c r="I7" s="16">
+        <v>123</v>
+      </c>
+      <c r="J7" s="16" t="s">
+        <v>32</v>
+      </c>
+      <c r="K7" s="38">
         <v>57.86</v>
       </c>
-      <c r="J6" s="40">
-        <f>I6-39.325-11</f>
+      <c r="L7" s="39">
+        <f>K7-39.325-11</f>
         <v>7.5349999999999966</v>
       </c>
-      <c r="K6" s="18">
+      <c r="M7" s="17">
         <v>167.12180000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="8">
-        <v>6</v>
-      </c>
-      <c r="B7" s="27">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" s="7">
+        <v>7</v>
+      </c>
+      <c r="B8" s="26">
         <v>9</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7" s="10">
+      <c r="C8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="9">
         <v>2</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F8" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="10" t="s">
+      <c r="G8" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="46">
+      <c r="H8" s="45">
         <v>12</v>
       </c>
-      <c r="I7" s="12">
+      <c r="I8" s="45">
+        <v>123</v>
+      </c>
+      <c r="J8" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K8" s="11">
         <v>55.279260000000001</v>
       </c>
-      <c r="J7" s="13">
-        <f>I7-39.325-11</f>
+      <c r="L8" s="12">
+        <f>K8-39.325-11</f>
         <v>4.9542599999999979</v>
       </c>
-      <c r="K7" s="15">
+      <c r="M8" s="14">
         <v>122.0548</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="36">
-        <v>6</v>
-      </c>
-      <c r="B8" s="47">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A9" s="7">
+        <v>8</v>
+      </c>
+      <c r="B9" s="26">
         <v>9</v>
       </c>
-      <c r="C8" s="37" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="37">
+      <c r="C9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="9">
+        <v>2</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" s="45">
+        <v>12</v>
+      </c>
+      <c r="I9" s="45">
+        <v>123</v>
+      </c>
+      <c r="J9" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="11">
+        <v>55.920229999999997</v>
+      </c>
+      <c r="L9" s="12">
+        <f>K9-39.325-11</f>
+        <v>5.5952299999999937</v>
+      </c>
+      <c r="M9" s="14">
+        <v>138.0641</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A10" s="7">
+        <v>9</v>
+      </c>
+      <c r="B10" s="26">
+        <v>9</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10" s="9">
+        <v>2</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="45">
+        <v>12</v>
+      </c>
+      <c r="I10" s="45">
+        <v>123</v>
+      </c>
+      <c r="J10" s="45" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="11">
+        <v>56.619590000000002</v>
+      </c>
+      <c r="L10" s="12">
+        <f>K10-39.325-11</f>
+        <v>6.2945899999999995</v>
+      </c>
+      <c r="M10" s="14">
+        <v>146.6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="49">
+        <v>10</v>
+      </c>
+      <c r="B11" s="55">
+        <v>9</v>
+      </c>
+      <c r="C11" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="50">
+        <v>2</v>
+      </c>
+      <c r="E11" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="51">
+        <v>12</v>
+      </c>
+      <c r="I11" s="51">
+        <v>123456</v>
+      </c>
+      <c r="J11" s="51" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="52">
+        <v>56.619590000000002</v>
+      </c>
+      <c r="L11" s="53">
+        <f>K11-39.325-11</f>
+        <v>6.2945899999999995</v>
+      </c>
+      <c r="M11" s="54">
+        <v>181.3417</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="15">
+        <v>11</v>
+      </c>
+      <c r="B12" s="56">
+        <v>9</v>
+      </c>
+      <c r="C12" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="16">
+        <v>2</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G12" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="57">
+        <v>12</v>
+      </c>
+      <c r="I12" s="57">
+        <v>123456</v>
+      </c>
+      <c r="J12" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="38">
+        <v>55.279260000000001</v>
+      </c>
+      <c r="L12" s="39">
+        <f>K12-39.325-11</f>
+        <v>4.9542599999999979</v>
+      </c>
+      <c r="M12" s="17">
+        <v>153.84200000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="7">
+        <v>12</v>
+      </c>
+      <c r="B13" s="26">
+        <v>9</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="9">
+        <v>2</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H13" s="45">
+        <v>8</v>
+      </c>
+      <c r="I13" s="45">
+        <v>123</v>
+      </c>
+      <c r="J13" s="45" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" s="11">
+        <v>53.23968</v>
+      </c>
+      <c r="L13" s="12">
+        <f>K13-39.325-11</f>
+        <v>2.9146799999999971</v>
+      </c>
+      <c r="M13" s="14">
+        <v>64.546589999999995</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="35">
+        <v>13</v>
+      </c>
+      <c r="B14" s="46">
+        <v>9</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="36">
         <v>3</v>
       </c>
-      <c r="E8" s="37" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="37" t="s">
+      <c r="E14" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="37" t="s">
+      <c r="G14" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="37">
-        <v>8</v>
-      </c>
-      <c r="I8" s="37"/>
-      <c r="J8" s="37"/>
-      <c r="K8" s="38">
+      <c r="H14" s="36">
+        <v>8</v>
+      </c>
+      <c r="I14" s="36">
+        <v>123</v>
+      </c>
+      <c r="J14" s="36" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="36"/>
+      <c r="L14" s="36"/>
+      <c r="M14" s="37">
         <v>169.4</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>7</v>
-      </c>
-      <c r="B9" s="26">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="25">
         <v>11</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="3">
         <v>2</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="E15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H9" s="3">
-        <v>8</v>
-      </c>
-      <c r="I9" s="5">
+      <c r="H15" s="2">
+        <v>8</v>
+      </c>
+      <c r="I15" s="2">
+        <v>123</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="4">
         <v>53.47</v>
       </c>
-      <c r="J9" s="6">
-        <f>I9-39.325-11</f>
+      <c r="L15" s="5">
+        <f>K15-39.325-11</f>
         <v>3.144999999999996</v>
       </c>
-      <c r="K9" s="7">
+      <c r="M15" s="6">
         <v>42.4</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="8">
-        <v>8</v>
-      </c>
-      <c r="B10" s="27">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="7">
+        <v>15</v>
+      </c>
+      <c r="B16" s="26">
         <v>11</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D10" s="11">
+      <c r="C16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="10">
         <v>2</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G10" s="10" t="s">
+      <c r="G16" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="10">
-        <v>8</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="25">
+      <c r="H16" s="9">
+        <v>8</v>
+      </c>
+      <c r="I16" s="9">
+        <v>123</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="12"/>
+      <c r="M16" s="24">
         <v>74.625</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="8">
-        <v>9</v>
-      </c>
-      <c r="B11" s="27">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>16</v>
+      </c>
+      <c r="B17" s="26">
         <v>11</v>
       </c>
-      <c r="C11" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" s="10">
+      <c r="C17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="9">
         <v>3</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F11" s="10" t="s">
+      <c r="E17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="G11" s="10" t="s">
+      <c r="G17" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="10">
-        <v>8</v>
-      </c>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="33">
+      <c r="H17" s="9">
+        <v>8</v>
+      </c>
+      <c r="I17" s="9">
+        <v>123</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K17" s="9"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="32">
         <v>91.368440000000007</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="8">
-        <v>10</v>
-      </c>
-      <c r="B12" s="27">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
+        <v>17</v>
+      </c>
+      <c r="B18" s="26">
         <v>11</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="10">
+      <c r="C18" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" s="9">
         <v>3</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="E18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="G18" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="H12" s="10">
-        <v>8</v>
-      </c>
-      <c r="I12" s="12">
+      <c r="H18" s="9">
+        <v>8</v>
+      </c>
+      <c r="I18" s="9">
+        <v>123</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="11">
         <v>56.938980000000001</v>
       </c>
-      <c r="J12" s="44">
-        <f>I12-39.325-11</f>
+      <c r="L18" s="43">
+        <f>K18-39.325-11</f>
         <v>6.613979999999998</v>
       </c>
-      <c r="K12" s="33">
+      <c r="M18" s="32">
         <v>90.916380000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="28">
+    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="27">
+        <v>18</v>
+      </c>
+      <c r="B19" s="28">
         <v>11</v>
       </c>
-      <c r="B13" s="29">
-        <v>11</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="10">
+      <c r="C19" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" s="9">
         <v>3</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="10" t="s">
+      <c r="E19" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G19" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="H13" s="10">
-        <v>8</v>
-      </c>
-      <c r="I13" s="42">
+      <c r="H19" s="9">
+        <v>8</v>
+      </c>
+      <c r="I19" s="48">
+        <v>123</v>
+      </c>
+      <c r="J19" s="48" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="41">
         <v>58.935200000000002</v>
       </c>
-      <c r="J13" s="43">
-        <f>I13-39.325-11</f>
+      <c r="L19" s="42">
+        <f>K19-39.325-11</f>
         <v>8.610199999999999</v>
       </c>
-      <c r="K13" s="41">
+      <c r="M19" s="40">
         <v>96.857420000000005</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="25">
+        <v>7</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="3">
+        <v>2</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="26">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H20" s="2">
+        <v>8</v>
+      </c>
+      <c r="I20" s="9">
+        <v>123</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K20" s="4">
+        <v>53.008029999999998</v>
+      </c>
+      <c r="L20" s="43">
+        <f>K20-39.325-11</f>
+        <v>2.6830299999999951</v>
+      </c>
+      <c r="M20" s="6">
+        <v>57.629820000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
+        <v>20</v>
+      </c>
+      <c r="B21" s="26">
+        <v>7</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" s="10">
         <v>2</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="3">
-        <v>8</v>
-      </c>
-      <c r="I14" s="5">
-        <v>53.008029999999998</v>
-      </c>
-      <c r="J14" s="44">
-        <f>I14-39.325-11</f>
-        <v>2.6830299999999951</v>
-      </c>
-      <c r="K14" s="7">
-        <v>57.629820000000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="8">
-        <v>13</v>
-      </c>
-      <c r="B15" s="27">
-        <v>7</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="11">
-        <v>2</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="10" t="s">
+      <c r="E21" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G21" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="10">
-        <v>8</v>
-      </c>
-      <c r="I15" s="10"/>
-      <c r="J15" s="13"/>
-      <c r="K15" s="25">
+      <c r="H21" s="9">
+        <v>8</v>
+      </c>
+      <c r="I21" s="9">
+        <v>123</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="9"/>
+      <c r="L21" s="12"/>
+      <c r="M21" s="24">
         <v>74.625</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="8">
-        <v>14</v>
-      </c>
-      <c r="B16" s="27">
-        <v>7</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="11">
-        <v>3</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H16" s="10">
-        <v>8</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="13"/>
-      <c r="K16" s="25">
-        <v>114.49639999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A17" s="8">
-        <v>15</v>
-      </c>
-      <c r="B17" s="27">
-        <v>7</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="11">
-        <v>3</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="G17" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="H17" s="10">
-        <v>8</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="25">
-        <v>128.84270000000001</v>
-      </c>
-      <c r="L17" s="34"/>
-      <c r="M17" s="34"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A18" s="8">
-        <v>16</v>
-      </c>
-      <c r="B18" s="27">
-        <v>7</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" s="11">
-        <v>3</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="G18" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="H18" s="10">
-        <v>8</v>
-      </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="13"/>
-      <c r="K18" s="35">
-        <v>95.542420000000007</v>
-      </c>
-      <c r="L18" s="34"/>
-      <c r="M18" s="34"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A19" s="8">
-        <v>17</v>
-      </c>
-      <c r="B19" s="27">
-        <v>7</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="D19" s="10">
-        <v>4</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="10">
-        <v>8</v>
-      </c>
-      <c r="I19" s="10"/>
-      <c r="J19" s="10"/>
-      <c r="K19" s="33">
-        <v>146.65029999999999</v>
-      </c>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="P19" s="45"/>
-    </row>
-    <row r="20" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="19">
-        <v>18</v>
-      </c>
-      <c r="B20" s="20">
-        <v>7</v>
-      </c>
-      <c r="C20" s="21" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="21">
-        <v>4</v>
-      </c>
-      <c r="E20" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" s="21" t="s">
-        <v>16</v>
-      </c>
-      <c r="G20" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="H20" s="21">
-        <v>8</v>
-      </c>
-      <c r="I20" s="31">
-        <v>58.475189999999998</v>
-      </c>
-      <c r="J20" s="32">
-        <f>I20-39.325-11</f>
-        <v>8.1501899999999949</v>
-      </c>
-      <c r="K20" s="30">
-        <v>154.22069999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="26">
-        <v>7</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="4">
-        <v>2</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="H21" s="10">
-        <v>8</v>
-      </c>
-      <c r="I21" s="12">
-        <v>54.569940000000003</v>
-      </c>
-      <c r="J21" s="13">
-        <f>I21-39.325-11</f>
-        <v>4.2449399999999997</v>
-      </c>
-      <c r="K21" s="7">
-        <v>72.7</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A22" s="8">
-        <v>20</v>
-      </c>
-      <c r="B22" s="27">
-        <v>7</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>28</v>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
+        <v>21</v>
+      </c>
+      <c r="B22" s="26">
+        <v>7</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>7</v>
       </c>
       <c r="D22" s="10">
         <v>3</v>
       </c>
-      <c r="E22" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" s="10" t="s">
+      <c r="E22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" s="9">
+        <v>8</v>
+      </c>
+      <c r="I22" s="9">
+        <v>123</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="12"/>
+      <c r="M22" s="24">
+        <v>114.49639999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
+        <v>22</v>
+      </c>
+      <c r="B23" s="26">
+        <v>7</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="10">
+        <v>3</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="H23" s="9">
+        <v>8</v>
+      </c>
+      <c r="I23" s="9">
+        <v>123</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="12"/>
+      <c r="M23" s="24">
+        <v>128.84270000000001</v>
+      </c>
+      <c r="N23" s="33"/>
+      <c r="O23" s="33"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A24" s="7">
+        <v>23</v>
+      </c>
+      <c r="B24" s="26">
+        <v>7</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" s="10">
+        <v>3</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H24" s="9">
+        <v>8</v>
+      </c>
+      <c r="I24" s="9">
+        <v>123</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="12"/>
+      <c r="M24" s="34">
+        <v>95.542420000000007</v>
+      </c>
+      <c r="N24" s="33"/>
+      <c r="O24" s="33"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A25" s="7">
+        <v>24</v>
+      </c>
+      <c r="B25" s="26">
+        <v>7</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="9">
+        <v>4</v>
+      </c>
+      <c r="E25" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="H25" s="9">
+        <v>8</v>
+      </c>
+      <c r="I25" s="9">
+        <v>123</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="32">
+        <v>146.65029999999999</v>
+      </c>
+      <c r="N25" s="33"/>
+      <c r="O25" s="33"/>
+      <c r="R25" s="44"/>
+    </row>
+    <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="18">
+        <v>25</v>
+      </c>
+      <c r="B26" s="19">
+        <v>7</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="20">
+        <v>4</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H26" s="20">
+        <v>8</v>
+      </c>
+      <c r="I26" s="20">
+        <v>123</v>
+      </c>
+      <c r="J26" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="K26" s="30">
+        <v>58.475189999999998</v>
+      </c>
+      <c r="L26" s="31">
+        <f>K26-39.325-11</f>
+        <v>8.1501899999999949</v>
+      </c>
+      <c r="M26" s="29">
+        <v>154.22069999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="25">
+        <v>7</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D27" s="3">
+        <v>2</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H27" s="9">
+        <v>8</v>
+      </c>
+      <c r="I27" s="9">
+        <v>123</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" s="11">
+        <v>54.569940000000003</v>
+      </c>
+      <c r="L27" s="12">
+        <f>K27-39.325-11</f>
+        <v>4.2449399999999997</v>
+      </c>
+      <c r="M27" s="6">
+        <v>72.7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A28" s="7">
+        <v>27</v>
+      </c>
+      <c r="B28" s="26">
+        <v>7</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D28" s="9">
+        <v>3</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G28" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H22" s="10">
-        <v>8</v>
-      </c>
-      <c r="I22" s="12">
+      <c r="H28" s="9">
+        <v>8</v>
+      </c>
+      <c r="I28" s="9">
+        <v>123</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="K28" s="11">
         <v>58.15</v>
       </c>
-      <c r="J22" s="13">
-        <f>I22-39.325-11</f>
+      <c r="L28" s="12">
+        <f>K28-39.325-11</f>
         <v>7.8249999999999957</v>
       </c>
-      <c r="K22" s="33">
+      <c r="M28" s="32">
         <v>135.0454</v>
       </c>
     </row>
@@ -1544,12 +1970,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="c5ae091c-4d86-42b7-bd6d-05a6d5850206">
+      <UserInfo>
+        <DisplayName>Integrantes de la CURSO 1º MUSE</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1718,23 +2149,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="c5ae091c-4d86-42b7-bd6d-05a6d5850206">
-      <UserInfo>
-        <DisplayName>Integrantes de la CURSO 1º MUSE</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A54CB81-BDC2-4F30-B8AA-8FF202FE488F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F2DDC3-8EF2-4F40-AEC5-CBD2E661EA55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5ae091c-4d86-42b7-bd6d-05a6d5850206"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1759,11 +2187,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F2DDC3-8EF2-4F40-AEC5-CBD2E661EA55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A54CB81-BDC2-4F30-B8AA-8FF202FE488F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5ae091c-4d86-42b7-bd6d-05a6d5850206"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Vamos con el analisis de sensibilidades
</commit_message>
<xml_diff>
--- a/MicroSat/Iteraciones.xlsx
+++ b/MicroSat/Iteraciones.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\MEng Space Systems (Local)\2. EUE\Micro-Satellite Design &amp; Analysis\MicroSat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B865522C-A394-4093-872B-BB5F3D6B500B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F544B92-6550-44D1-97F2-F743E04353CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="It_Bandeja Inf" sheetId="1" r:id="rId1"/>
+    <sheet name="Analisis de Sensibilidad" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="78">
   <si>
     <t>Nº rigidizadores</t>
   </si>
@@ -126,9 +127,6 @@
     <t>CBUSH (number)</t>
   </si>
   <si>
-    <t>RBE2 DOF</t>
-  </si>
-  <si>
     <t>Posición RBE2 Mequip</t>
   </si>
   <si>
@@ -136,6 +134,141 @@
   </si>
   <si>
     <t>Alejado</t>
+  </si>
+  <si>
+    <t>RBE2 restricted DOF</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Espesor bandeja</t>
+  </si>
+  <si>
+    <t>Sección rigidizadores int</t>
+  </si>
+  <si>
+    <t>Los valores de masa que me comentas son altos (en el UPMSat-2 eran de</t>
+  </si>
+  <si>
+    <t>&gt; 3 kg), así que conviene buscar formas de conseguir reducir esa masa.</t>
+  </si>
+  <si>
+    <t>&gt; Te recomiendo que hagas un análisis de sensibilidad, variando cada vez</t>
+  </si>
+  <si>
+    <t>&gt; uno de los parámetros y cuantificar cómo han variado la masa y los</t>
+  </si>
+  <si>
+    <t>&gt; resultados (frecuencias o tensiones máximas). De esa forma, puedes</t>
+  </si>
+  <si>
+    <t>&gt; hacer una comparativa entre los diferentes parámetros para decidir</t>
+  </si>
+  <si>
+    <t>&gt; cuál merece la pena variar más para conseguir minimizar la masa y</t>
+  </si>
+  <si>
+    <t>&gt; cumplir los requisitos estructurales.</t>
+  </si>
+  <si>
+    <t>Iteración Referencia</t>
+  </si>
+  <si>
+    <t>Iteración 1</t>
+  </si>
+  <si>
+    <t>Iteración 2</t>
+  </si>
+  <si>
+    <t>% Change itref-it1</t>
+  </si>
+  <si>
+    <t>% Change itref-it2</t>
+  </si>
+  <si>
+    <t>MoS</t>
+  </si>
+  <si>
+    <t>Mass [kg]</t>
+  </si>
+  <si>
+    <t>fn [Hz]</t>
+  </si>
+  <si>
+    <t>Elem. CBUSH</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>MoS_vonmisses</t>
+  </si>
+  <si>
+    <t>0&lt;=MoS&lt;=0.5</t>
+  </si>
+  <si>
+    <t>150&lt;=fn &lt;=175</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Proceso:</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Variar solo una variable a la vez</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>Al-7075 T6</t>
+  </si>
+  <si>
+    <t>CFRP</t>
+  </si>
+  <si>
+    <t>DOF RBE2</t>
+  </si>
+  <si>
+    <t>Debería modificar todo a partir de un solo archivo, para que el resto de parámetros sean constantes</t>
+  </si>
+  <si>
+    <t>fn [%]</t>
+  </si>
+  <si>
+    <t>Mass [%]</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Dim. Rig. Int. x [mm]</t>
+  </si>
+  <si>
+    <t>Dim. Rig. Int. z [mm]</t>
+  </si>
+  <si>
+    <t>Dim. Rig. Ext. x [mm]</t>
+  </si>
+  <si>
+    <t>Dim. Rig. Ext. z [mm]</t>
+  </si>
+  <si>
+    <t>20 COMBINACIONES!!</t>
+  </si>
+  <si>
+    <t>MicroSat\It1_9rig\Sat_Bandeja_Inf_9rig_rect_Al7075_3mm_19x13_19x9.5_12CBUSH</t>
+  </si>
+  <si>
+    <t>Configuración / Archivo empleado IT1</t>
+  </si>
+  <si>
+    <t>Configuración / Archivo empleado IT2</t>
   </si>
 </sst>
 </file>
@@ -147,7 +280,7 @@
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +324,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,8 +362,60 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="40">
     <border>
       <left/>
       <right/>
@@ -347,15 +540,374 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -524,10 +1076,447 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="30" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="17" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="28" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="27" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="28" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="30" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="17" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="29" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="28" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="20" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="4" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="25" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="22" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="28" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="20" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="27" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="30" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="17" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="29" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="28" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="27" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="13" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="26" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="33" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="34" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="35" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="33" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="34" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="35" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="33" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="34" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="35" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="33" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="34" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="35" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="33" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="34" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="25" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="36" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="1" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="6" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="28" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="29" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="30" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="17" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="29" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="17" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="5" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="20" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="27" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="28" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="20" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="27" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="27" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="20" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="4" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="23" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="24" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="23" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="24" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="4" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="5" xfId="8" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="22" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="23" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="24" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="22" xfId="7" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="7" borderId="22" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="23" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="23" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="24" xfId="6" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="22" xfId="12" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="12" borderId="22" xfId="11" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="23" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="14">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent3" xfId="9" builtinId="38"/>
+    <cellStyle name="20% - Accent4" xfId="11" builtinId="42"/>
+    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
+    <cellStyle name="40% - Accent4" xfId="12" builtinId="43"/>
     <cellStyle name="40% - Accent6" xfId="4" builtinId="51"/>
+    <cellStyle name="60% - Accent2" xfId="7" builtinId="36"/>
+    <cellStyle name="60% - Accent3" xfId="10" builtinId="40"/>
+    <cellStyle name="60% - Accent4" xfId="13" builtinId="44"/>
+    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Accent3" xfId="8" builtinId="37"/>
     <cellStyle name="Accent5" xfId="2" builtinId="45"/>
     <cellStyle name="Accent6" xfId="3" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -808,10 +1797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R28"/>
+  <dimension ref="A1:R30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P29" sqref="P29"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15:H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -822,9 +1811,10 @@
     <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.33203125" customWidth="1"/>
     <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="8" width="10.5546875" customWidth="1"/>
-    <col min="9" max="9" width="7.88671875" customWidth="1"/>
-    <col min="10" max="10" width="8.5546875" customWidth="1"/>
+    <col min="7" max="7" width="10.5546875" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="9.44140625" customWidth="1"/>
     <col min="11" max="11" width="10.5546875" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
     <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
@@ -856,10 +1846,10 @@
         <v>29</v>
       </c>
       <c r="I1" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>30</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>31</v>
       </c>
       <c r="K1" s="22" t="s">
         <v>4</v>
@@ -900,7 +1890,7 @@
         <v>123</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K2" s="11">
         <v>53.24</v>
@@ -942,7 +1932,7 @@
         <v>123456</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K3" s="11">
         <v>53.24</v>
@@ -984,7 +1974,7 @@
         <v>123</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="12"/>
@@ -1021,7 +2011,7 @@
         <v>123</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
@@ -1029,7 +2019,7 @@
         <v>119.2757</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15">
         <v>5</v>
       </c>
@@ -1058,23 +2048,21 @@
         <v>123</v>
       </c>
       <c r="J6" s="16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K6" s="38">
         <v>57.86</v>
       </c>
       <c r="L6" s="39">
-        <f>K6-39.325-11</f>
+        <f t="shared" ref="L6:L15" si="0">K6-39.325-11</f>
         <v>7.5349999999999966</v>
       </c>
       <c r="M6" s="17">
         <v>152.38999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="15">
-        <v>6</v>
-      </c>
+    <row r="7" spans="1:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15"/>
       <c r="B7" s="47">
         <v>9</v>
       </c>
@@ -1088,10 +2076,10 @@
         <v>10</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>16</v>
+        <v>25</v>
       </c>
       <c r="H7" s="16">
         <v>12</v>
@@ -1100,106 +2088,74 @@
         <v>123</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="K7" s="38">
+        <v>31</v>
+      </c>
+      <c r="K7" s="38"/>
+      <c r="L7" s="39"/>
+      <c r="M7" s="17">
+        <v>156.0129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="16"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="16"/>
+      <c r="K8" s="38"/>
+      <c r="L8" s="39"/>
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" spans="1:13" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
+        <v>6</v>
+      </c>
+      <c r="B9" s="47">
+        <v>9</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="16">
+        <v>3</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="16">
+        <v>12</v>
+      </c>
+      <c r="I9" s="16">
+        <v>123</v>
+      </c>
+      <c r="J9" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="K9" s="38">
         <v>57.86</v>
       </c>
-      <c r="L7" s="39">
-        <f>K7-39.325-11</f>
+      <c r="L9" s="39">
+        <f t="shared" si="0"/>
         <v>7.5349999999999966</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M9" s="17">
         <v>167.12180000000001</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="7">
-        <v>7</v>
-      </c>
-      <c r="B8" s="26">
-        <v>9</v>
-      </c>
-      <c r="C8" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="9">
-        <v>2</v>
-      </c>
-      <c r="E8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="45">
-        <v>12</v>
-      </c>
-      <c r="I8" s="45">
-        <v>123</v>
-      </c>
-      <c r="J8" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="K8" s="11">
-        <v>55.279260000000001</v>
-      </c>
-      <c r="L8" s="12">
-        <f>K8-39.325-11</f>
-        <v>4.9542599999999979</v>
-      </c>
-      <c r="M8" s="14">
-        <v>122.0548</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="7">
-        <v>8</v>
-      </c>
-      <c r="B9" s="26">
-        <v>9</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D9" s="9">
-        <v>2</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="H9" s="45">
-        <v>12</v>
-      </c>
-      <c r="I9" s="45">
-        <v>123</v>
-      </c>
-      <c r="J9" s="45" t="s">
-        <v>32</v>
-      </c>
-      <c r="K9" s="11">
-        <v>55.920229999999997</v>
-      </c>
-      <c r="L9" s="12">
-        <f>K9-39.325-11</f>
-        <v>5.5952299999999937</v>
-      </c>
-      <c r="M9" s="14">
-        <v>138.0641</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B10" s="26">
         <v>9</v>
@@ -1214,10 +2170,10 @@
         <v>10</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="H10" s="45">
         <v>12</v>
@@ -1226,301 +2182,311 @@
         <v>123</v>
       </c>
       <c r="J10" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="K10" s="11">
+        <v>55.279260000000001</v>
+      </c>
+      <c r="L10" s="12">
+        <f t="shared" si="0"/>
+        <v>4.9542599999999979</v>
+      </c>
+      <c r="M10" s="14">
+        <v>122.0548</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="26">
+        <v>9</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="9">
+        <v>2</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="45">
+        <v>12</v>
+      </c>
+      <c r="I11" s="45">
+        <v>123</v>
+      </c>
+      <c r="J11" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="11">
+        <v>55.920229999999997</v>
+      </c>
+      <c r="L11" s="12">
+        <f t="shared" si="0"/>
+        <v>5.5952299999999937</v>
+      </c>
+      <c r="M11" s="14">
+        <v>138.0641</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="7">
+        <v>9</v>
+      </c>
+      <c r="B12" s="26">
+        <v>9</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" s="9">
+        <v>2</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="45">
+        <v>12</v>
+      </c>
+      <c r="I12" s="45">
+        <v>123</v>
+      </c>
+      <c r="J12" s="45" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="11">
+        <v>56.619590000000002</v>
+      </c>
+      <c r="L12" s="12">
+        <f t="shared" si="0"/>
+        <v>6.2945899999999995</v>
+      </c>
+      <c r="M12" s="14">
+        <v>146.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" s="49">
+        <v>10</v>
+      </c>
+      <c r="B13" s="55">
+        <v>9</v>
+      </c>
+      <c r="C13" s="50" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="50">
+        <v>2</v>
+      </c>
+      <c r="E13" s="50" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="50" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="50" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="51">
+        <v>12</v>
+      </c>
+      <c r="I13" s="51">
+        <v>123456</v>
+      </c>
+      <c r="J13" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="52">
+        <v>56.619590000000002</v>
+      </c>
+      <c r="L13" s="53">
+        <f t="shared" si="0"/>
+        <v>6.2945899999999995</v>
+      </c>
+      <c r="M13" s="54">
+        <v>181.3417</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
+        <v>11</v>
+      </c>
+      <c r="B14" s="56">
+        <v>9</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="16">
+        <v>2</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H14" s="57">
+        <v>12</v>
+      </c>
+      <c r="I14" s="57">
+        <v>123456</v>
+      </c>
+      <c r="J14" s="57" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="38">
+        <v>55.279260000000001</v>
+      </c>
+      <c r="L14" s="39">
+        <f t="shared" si="0"/>
+        <v>4.9542599999999979</v>
+      </c>
+      <c r="M14" s="17">
+        <v>153.84200000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="7">
+        <v>12</v>
+      </c>
+      <c r="B15" s="26">
+        <v>9</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" s="9">
+        <v>2</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="45">
+        <v>8</v>
+      </c>
+      <c r="I15" s="45">
+        <v>123</v>
+      </c>
+      <c r="J15" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="K10" s="11">
-        <v>56.619590000000002</v>
-      </c>
-      <c r="L10" s="12">
-        <f>K10-39.325-11</f>
-        <v>6.2945899999999995</v>
-      </c>
-      <c r="M10" s="14">
-        <v>146.6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="49">
+      <c r="K15" s="11">
+        <v>53.23968</v>
+      </c>
+      <c r="L15" s="12">
+        <f t="shared" si="0"/>
+        <v>2.9146799999999971</v>
+      </c>
+      <c r="M15" s="14">
+        <v>64.546589999999995</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="35">
+        <v>13</v>
+      </c>
+      <c r="B16" s="46">
+        <v>9</v>
+      </c>
+      <c r="C16" s="36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="36">
+        <v>3</v>
+      </c>
+      <c r="E16" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="55">
-        <v>9</v>
-      </c>
-      <c r="C11" s="50" t="s">
+      <c r="F16" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="36">
+        <v>8</v>
+      </c>
+      <c r="I16" s="36">
+        <v>123</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="36"/>
+      <c r="L16" s="36"/>
+      <c r="M16" s="37">
+        <v>169.4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>14</v>
+      </c>
+      <c r="B17" s="25">
+        <v>11</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="50">
+      <c r="D17" s="3">
         <v>2</v>
       </c>
-      <c r="E11" s="50" t="s">
+      <c r="E17" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F11" s="50" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="50" t="s">
-        <v>16</v>
-      </c>
-      <c r="H11" s="51">
+      <c r="F17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="51">
-        <v>123456</v>
-      </c>
-      <c r="J11" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="52">
-        <v>56.619590000000002</v>
-      </c>
-      <c r="L11" s="53">
-        <f>K11-39.325-11</f>
-        <v>6.2945899999999995</v>
-      </c>
-      <c r="M11" s="54">
-        <v>181.3417</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" s="15">
-        <v>11</v>
-      </c>
-      <c r="B12" s="56">
-        <v>9</v>
-      </c>
-      <c r="C12" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" s="16">
-        <v>2</v>
-      </c>
-      <c r="E12" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>21</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>23</v>
-      </c>
-      <c r="H12" s="57">
-        <v>12</v>
-      </c>
-      <c r="I12" s="57">
-        <v>123456</v>
-      </c>
-      <c r="J12" s="57" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="38">
-        <v>55.279260000000001</v>
-      </c>
-      <c r="L12" s="39">
-        <f>K12-39.325-11</f>
-        <v>4.9542599999999979</v>
-      </c>
-      <c r="M12" s="17">
-        <v>153.84200000000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="7">
-        <v>12</v>
-      </c>
-      <c r="B13" s="26">
-        <v>9</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="9">
-        <v>2</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" s="9" t="s">
+      <c r="G17" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H13" s="45">
+      <c r="H17" s="2">
         <v>8</v>
       </c>
-      <c r="I13" s="45">
+      <c r="I17" s="2">
         <v>123</v>
       </c>
-      <c r="J13" s="45" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="11">
-        <v>53.23968</v>
-      </c>
-      <c r="L13" s="12">
-        <f>K13-39.325-11</f>
-        <v>2.9146799999999971</v>
-      </c>
-      <c r="M13" s="14">
-        <v>64.546589999999995</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="35">
-        <v>13</v>
-      </c>
-      <c r="B14" s="46">
-        <v>9</v>
-      </c>
-      <c r="C14" s="36" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" s="36">
-        <v>3</v>
-      </c>
-      <c r="E14" s="36" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="36">
-        <v>8</v>
-      </c>
-      <c r="I14" s="36">
-        <v>123</v>
-      </c>
-      <c r="J14" s="36" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="36"/>
-      <c r="L14" s="36"/>
-      <c r="M14" s="37">
-        <v>169.4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
-        <v>14</v>
-      </c>
-      <c r="B15" s="25">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D15" s="3">
-        <v>2</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H15" s="2">
-        <v>8</v>
-      </c>
-      <c r="I15" s="2">
-        <v>123</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="4">
+      <c r="J17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="4">
         <v>53.47</v>
       </c>
-      <c r="L15" s="5">
-        <f>K15-39.325-11</f>
+      <c r="L17" s="5">
+        <f>K17-39.325-11</f>
         <v>3.144999999999996</v>
       </c>
-      <c r="M15" s="6">
+      <c r="M17" s="6">
         <v>42.4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="7">
-        <v>15</v>
-      </c>
-      <c r="B16" s="26">
-        <v>11</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D16" s="10">
-        <v>2</v>
-      </c>
-      <c r="E16" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="H16" s="9">
-        <v>8</v>
-      </c>
-      <c r="I16" s="9">
-        <v>123</v>
-      </c>
-      <c r="J16" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="24">
-        <v>74.625</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A17" s="7">
-        <v>16</v>
-      </c>
-      <c r="B17" s="26">
-        <v>11</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="D17" s="9">
-        <v>3</v>
-      </c>
-      <c r="E17" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="G17" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H17" s="9">
-        <v>8</v>
-      </c>
-      <c r="I17" s="9">
-        <v>123</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="32">
-        <v>91.368440000000007</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" s="26">
         <v>11</v>
@@ -1528,17 +2494,17 @@
       <c r="C18" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D18" s="9">
-        <v>3</v>
+      <c r="D18" s="10">
+        <v>2</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H18" s="9">
         <v>8</v>
@@ -1547,24 +2513,19 @@
         <v>123</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K18" s="11">
-        <v>56.938980000000001</v>
-      </c>
-      <c r="L18" s="43">
-        <f>K18-39.325-11</f>
-        <v>6.613979999999998</v>
-      </c>
-      <c r="M18" s="32">
-        <v>90.916380000000004</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="27">
-        <v>18</v>
-      </c>
-      <c r="B19" s="28">
+        <v>31</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="24">
+        <v>74.625</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
+        <v>16</v>
+      </c>
+      <c r="B19" s="26">
         <v>11</v>
       </c>
       <c r="C19" s="9" t="s">
@@ -1577,150 +2538,155 @@
         <v>10</v>
       </c>
       <c r="F19" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="G19" s="9" t="s">
-        <v>26</v>
       </c>
       <c r="H19" s="9">
         <v>8</v>
       </c>
-      <c r="I19" s="48">
+      <c r="I19" s="9">
         <v>123</v>
       </c>
-      <c r="J19" s="48" t="s">
-        <v>32</v>
-      </c>
-      <c r="K19" s="41">
-        <v>58.935200000000002</v>
-      </c>
-      <c r="L19" s="42">
-        <f>K19-39.325-11</f>
-        <v>8.610199999999999</v>
-      </c>
-      <c r="M19" s="40">
-        <v>96.857420000000005</v>
+      <c r="J19" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="32">
+        <v>91.368440000000007</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>19</v>
-      </c>
-      <c r="B20" s="25">
+      <c r="A20" s="7">
+        <v>17</v>
+      </c>
+      <c r="B20" s="26">
+        <v>11</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D20" s="3">
-        <v>2</v>
-      </c>
-      <c r="E20" s="2" t="s">
+      <c r="D20" s="9">
+        <v>3</v>
+      </c>
+      <c r="E20" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H20" s="2">
+      <c r="F20" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="H20" s="9">
         <v>8</v>
       </c>
       <c r="I20" s="9">
         <v>123</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="4">
-        <v>53.008029999999998</v>
+        <v>31</v>
+      </c>
+      <c r="K20" s="11">
+        <v>56.938980000000001</v>
       </c>
       <c r="L20" s="43">
         <f>K20-39.325-11</f>
-        <v>2.6830299999999951</v>
-      </c>
-      <c r="M20" s="6">
-        <v>57.629820000000002</v>
-      </c>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A21" s="7">
-        <v>20</v>
-      </c>
-      <c r="B21" s="26">
-        <v>7</v>
+        <v>6.613979999999998</v>
+      </c>
+      <c r="M20" s="32">
+        <v>90.916380000000004</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="27">
+        <v>18</v>
+      </c>
+      <c r="B21" s="28">
+        <v>11</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D21" s="10">
-        <v>2</v>
+      <c r="D21" s="9">
+        <v>3</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="G21" s="9" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="H21" s="9">
         <v>8</v>
       </c>
-      <c r="I21" s="9">
+      <c r="I21" s="48">
         <v>123</v>
       </c>
-      <c r="J21" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="12"/>
-      <c r="M21" s="24">
-        <v>74.625</v>
+      <c r="J21" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="41">
+        <v>58.935200000000002</v>
+      </c>
+      <c r="L21" s="42">
+        <f>K21-39.325-11</f>
+        <v>8.610199999999999</v>
+      </c>
+      <c r="M21" s="40">
+        <v>96.857420000000005</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A22" s="7">
-        <v>21</v>
-      </c>
-      <c r="B22" s="26">
+      <c r="A22" s="1">
+        <v>19</v>
+      </c>
+      <c r="B22" s="25">
         <v>7</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C22" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D22" s="10">
-        <v>3</v>
-      </c>
-      <c r="E22" s="9" t="s">
+      <c r="D22" s="3">
+        <v>2</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F22" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" s="9">
+      <c r="F22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H22" s="2">
         <v>8</v>
       </c>
       <c r="I22" s="9">
         <v>123</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="24">
-        <v>114.49639999999999</v>
+        <v>31</v>
+      </c>
+      <c r="K22" s="4">
+        <v>53.008029999999998</v>
+      </c>
+      <c r="L22" s="43">
+        <f>K22-39.325-11</f>
+        <v>2.6830299999999951</v>
+      </c>
+      <c r="M22" s="6">
+        <v>57.629820000000002</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="7">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" s="26">
         <v>7</v>
@@ -1729,16 +2695,16 @@
         <v>7</v>
       </c>
       <c r="D23" s="10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H23" s="9">
         <v>8</v>
@@ -1747,19 +2713,17 @@
         <v>123</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="11"/>
+        <v>31</v>
+      </c>
+      <c r="K23" s="9"/>
       <c r="L23" s="12"/>
       <c r="M23" s="24">
-        <v>128.84270000000001</v>
-      </c>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
+        <v>74.625</v>
+      </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="7">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" s="26">
         <v>7</v>
@@ -1771,7 +2735,7 @@
         <v>3</v>
       </c>
       <c r="E24" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>23</v>
@@ -1786,19 +2750,17 @@
         <v>123</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K24" s="11"/>
       <c r="L24" s="12"/>
-      <c r="M24" s="34">
-        <v>95.542420000000007</v>
-      </c>
-      <c r="N24" s="33"/>
-      <c r="O24" s="33"/>
+      <c r="M24" s="24">
+        <v>114.49639999999999</v>
+      </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" s="26">
         <v>7</v>
@@ -1806,17 +2768,17 @@
       <c r="C25" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D25" s="9">
-        <v>4</v>
+      <c r="D25" s="10">
+        <v>3</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="G25" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H25" s="9">
         <v>8</v>
@@ -1825,80 +2787,76 @@
         <v>123</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-      <c r="M25" s="32">
-        <v>146.65029999999999</v>
+        <v>31</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="12"/>
+      <c r="M25" s="24">
+        <v>128.84270000000001</v>
       </c>
       <c r="N25" s="33"/>
       <c r="O25" s="33"/>
-      <c r="R25" s="44"/>
-    </row>
-    <row r="26" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="18">
-        <v>25</v>
-      </c>
-      <c r="B26" s="19">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A26" s="7">
+        <v>23</v>
+      </c>
+      <c r="B26" s="26">
         <v>7</v>
       </c>
-      <c r="C26" s="20" t="s">
+      <c r="C26" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D26" s="20">
+      <c r="D26" s="10">
+        <v>3</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H26" s="9">
+        <v>8</v>
+      </c>
+      <c r="I26" s="9">
+        <v>123</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="12"/>
+      <c r="M26" s="34">
+        <v>95.542420000000007</v>
+      </c>
+      <c r="N26" s="33"/>
+      <c r="O26" s="33"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A27" s="7">
+        <v>24</v>
+      </c>
+      <c r="B27" s="26">
+        <v>7</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" s="9">
         <v>4</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E27" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F26" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="G26" s="20" t="s">
+      <c r="F27" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G27" s="9" t="s">
         <v>20</v>
-      </c>
-      <c r="H26" s="20">
-        <v>8</v>
-      </c>
-      <c r="I26" s="20">
-        <v>123</v>
-      </c>
-      <c r="J26" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="30">
-        <v>58.475189999999998</v>
-      </c>
-      <c r="L26" s="31">
-        <f>K26-39.325-11</f>
-        <v>8.1501899999999949</v>
-      </c>
-      <c r="M26" s="29">
-        <v>154.22069999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A27" s="1">
-        <v>26</v>
-      </c>
-      <c r="B27" s="25">
-        <v>7</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D27" s="3">
-        <v>2</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F27" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>13</v>
       </c>
       <c r="H27" s="9">
         <v>8</v>
@@ -1907,58 +2865,140 @@
         <v>123</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K27" s="11">
+        <v>31</v>
+      </c>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="32">
+        <v>146.65029999999999</v>
+      </c>
+      <c r="N27" s="33"/>
+      <c r="O27" s="33"/>
+      <c r="R27" s="44"/>
+    </row>
+    <row r="28" spans="1:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="18">
+        <v>25</v>
+      </c>
+      <c r="B28" s="19">
+        <v>7</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="20">
+        <v>4</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F28" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="G28" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="H28" s="20">
+        <v>8</v>
+      </c>
+      <c r="I28" s="20">
+        <v>123</v>
+      </c>
+      <c r="J28" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="K28" s="30">
+        <v>58.475189999999998</v>
+      </c>
+      <c r="L28" s="31">
+        <f>K28-39.325-11</f>
+        <v>8.1501899999999949</v>
+      </c>
+      <c r="M28" s="29">
+        <v>154.22069999999999</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>26</v>
+      </c>
+      <c r="B29" s="25">
+        <v>7</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H29" s="9">
+        <v>8</v>
+      </c>
+      <c r="I29" s="9">
+        <v>123</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K29" s="11">
         <v>54.569940000000003</v>
       </c>
-      <c r="L27" s="12">
-        <f>K27-39.325-11</f>
+      <c r="L29" s="12">
+        <f>K29-39.325-11</f>
         <v>4.2449399999999997</v>
       </c>
-      <c r="M27" s="6">
+      <c r="M29" s="6">
         <v>72.7</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A28" s="7">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A30" s="7">
         <v>27</v>
       </c>
-      <c r="B28" s="26">
+      <c r="B30" s="26">
         <v>7</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D30" s="9">
         <v>3</v>
       </c>
-      <c r="E28" s="9" t="s">
+      <c r="E30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="9" t="s">
+      <c r="F30" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H30" s="9">
         <v>8</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I30" s="9">
         <v>123</v>
       </c>
-      <c r="J28" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="11">
+      <c r="J30" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="K30" s="11">
         <v>58.15</v>
       </c>
-      <c r="L28" s="12">
-        <f>K28-39.325-11</f>
+      <c r="L30" s="12">
+        <f>K30-39.325-11</f>
         <v>7.8249999999999957</v>
       </c>
-      <c r="M28" s="32">
+      <c r="M30" s="32">
         <v>135.0454</v>
       </c>
     </row>
@@ -1969,18 +3009,900 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519799BC-EE76-4C42-A73D-AC4D7E6854EE}">
+  <dimension ref="A1:AC29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="U12" sqref="U12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16" customWidth="1"/>
+    <col min="2" max="3" width="9.77734375" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" customWidth="1"/>
+    <col min="6" max="6" width="9.5546875" customWidth="1"/>
+    <col min="9" max="9" width="9.44140625" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.44140625" customWidth="1"/>
+    <col min="17" max="17" width="9.33203125" customWidth="1"/>
+    <col min="21" max="21" width="9.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="139" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="125" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="126"/>
+      <c r="D1" s="126"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="128" t="s">
+        <v>46</v>
+      </c>
+      <c r="G1" s="129"/>
+      <c r="H1" s="129"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="131" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="132"/>
+      <c r="L1" s="132"/>
+      <c r="M1" s="133"/>
+      <c r="N1" s="134" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" s="135"/>
+      <c r="P1" s="135"/>
+      <c r="Q1" s="136"/>
+      <c r="R1" s="137" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="138"/>
+      <c r="T1" s="138"/>
+      <c r="U1" s="138"/>
+      <c r="V1" s="196" t="s">
+        <v>76</v>
+      </c>
+      <c r="W1" s="197"/>
+      <c r="X1" s="197"/>
+      <c r="Y1" s="198"/>
+      <c r="Z1" s="196" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA1" s="197"/>
+      <c r="AB1" s="197"/>
+      <c r="AC1" s="198"/>
+    </row>
+    <row r="2" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="140"/>
+      <c r="B2" s="92" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="93" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="93" t="s">
+        <v>50</v>
+      </c>
+      <c r="E2" s="94" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="95" t="s">
+        <v>62</v>
+      </c>
+      <c r="G2" s="96" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="96" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" s="97" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" s="98" t="s">
+        <v>62</v>
+      </c>
+      <c r="K2" s="99" t="s">
+        <v>67</v>
+      </c>
+      <c r="L2" s="99" t="s">
+        <v>50</v>
+      </c>
+      <c r="M2" s="100" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="101" t="s">
+        <v>62</v>
+      </c>
+      <c r="O2" s="102" t="s">
+        <v>52</v>
+      </c>
+      <c r="P2" s="102" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q2" s="103" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" s="104" t="s">
+        <v>62</v>
+      </c>
+      <c r="S2" s="105" t="s">
+        <v>67</v>
+      </c>
+      <c r="T2" s="105" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="115" t="s">
+        <v>68</v>
+      </c>
+      <c r="V2" s="199"/>
+      <c r="W2" s="200"/>
+      <c r="X2" s="200"/>
+      <c r="Y2" s="201"/>
+      <c r="Z2" s="199"/>
+      <c r="AA2" s="200"/>
+      <c r="AB2" s="200"/>
+      <c r="AC2" s="201"/>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A3" s="77" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="71">
+        <v>9</v>
+      </c>
+      <c r="C3" s="72">
+        <v>152.4</v>
+      </c>
+      <c r="D3" s="72"/>
+      <c r="E3" s="73">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F3" s="83">
+        <v>7</v>
+      </c>
+      <c r="G3" s="84"/>
+      <c r="H3" s="84"/>
+      <c r="I3" s="85"/>
+      <c r="J3" s="65"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="154">
+        <v>11</v>
+      </c>
+      <c r="O3" s="155"/>
+      <c r="P3" s="155"/>
+      <c r="Q3" s="156"/>
+      <c r="R3" s="157"/>
+      <c r="S3" s="158"/>
+      <c r="T3" s="158"/>
+      <c r="U3" s="158"/>
+      <c r="V3" s="122"/>
+      <c r="W3" s="123"/>
+      <c r="X3" s="123"/>
+      <c r="Y3" s="124"/>
+      <c r="Z3" s="122"/>
+      <c r="AA3" s="123"/>
+      <c r="AB3" s="123"/>
+      <c r="AC3" s="124"/>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A4" s="106" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="107" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" s="108">
+        <v>152.4</v>
+      </c>
+      <c r="D4" s="108"/>
+      <c r="E4" s="109">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F4" s="110" t="s">
+        <v>64</v>
+      </c>
+      <c r="G4" s="111"/>
+      <c r="H4" s="111"/>
+      <c r="I4" s="112"/>
+      <c r="J4" s="113" t="s">
+        <v>60</v>
+      </c>
+      <c r="K4" s="114">
+        <f>(G4-C4)/C4*100</f>
+        <v>-100</v>
+      </c>
+      <c r="L4" s="114" t="e">
+        <f t="shared" ref="L4:M12" si="0">(H4-D4)/D4*100</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M4" s="114">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N4" s="159" t="s">
+        <v>60</v>
+      </c>
+      <c r="O4" s="160"/>
+      <c r="P4" s="160"/>
+      <c r="Q4" s="161"/>
+      <c r="R4" s="162" t="s">
+        <v>60</v>
+      </c>
+      <c r="S4" s="163">
+        <f>(O4-C4)/C4</f>
+        <v>-1</v>
+      </c>
+      <c r="T4" s="163" t="e">
+        <f t="shared" ref="T4:U12" si="1">(P4-D4)/D4</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U4" s="163">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="V4" s="122"/>
+      <c r="W4" s="123"/>
+      <c r="X4" s="123"/>
+      <c r="Y4" s="124"/>
+      <c r="Z4" s="122"/>
+      <c r="AA4" s="123"/>
+      <c r="AB4" s="123"/>
+      <c r="AC4" s="124"/>
+    </row>
+    <row r="5" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="78" t="s">
+        <v>36</v>
+      </c>
+      <c r="B5" s="74" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="90">
+        <v>152.4</v>
+      </c>
+      <c r="D5" s="90"/>
+      <c r="E5" s="91">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F5" s="86" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="87"/>
+      <c r="H5" s="87"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="67"/>
+      <c r="K5" s="68">
+        <f t="shared" ref="K5:K12" si="2">(G5-C5)/C5*100</f>
+        <v>-100</v>
+      </c>
+      <c r="L5" s="68" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M5" s="69">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N5" s="145" t="s">
+        <v>69</v>
+      </c>
+      <c r="O5" s="164"/>
+      <c r="P5" s="164"/>
+      <c r="Q5" s="165"/>
+      <c r="R5" s="166"/>
+      <c r="S5" s="167">
+        <f t="shared" ref="S5:S12" si="3">(O5-C5)/C5</f>
+        <v>-1</v>
+      </c>
+      <c r="T5" s="167" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U5" s="167">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="V5" s="122"/>
+      <c r="W5" s="123"/>
+      <c r="X5" s="123"/>
+      <c r="Y5" s="124"/>
+      <c r="Z5" s="122"/>
+      <c r="AA5" s="123"/>
+      <c r="AB5" s="123"/>
+      <c r="AC5" s="124"/>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A6" s="78" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="80">
+        <v>3</v>
+      </c>
+      <c r="C6" s="81">
+        <v>152.4</v>
+      </c>
+      <c r="D6" s="81"/>
+      <c r="E6" s="82">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F6" s="67">
+        <v>2</v>
+      </c>
+      <c r="G6" s="68"/>
+      <c r="H6" s="68"/>
+      <c r="I6" s="69"/>
+      <c r="J6" s="70"/>
+      <c r="K6" s="89">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+      <c r="L6" s="89" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M6" s="168">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N6" s="166">
+        <v>4</v>
+      </c>
+      <c r="O6" s="167"/>
+      <c r="P6" s="167"/>
+      <c r="Q6" s="169"/>
+      <c r="R6" s="170"/>
+      <c r="S6" s="171">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="T6" s="171" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U6" s="171">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="V6" s="122"/>
+      <c r="W6" s="123"/>
+      <c r="X6" s="123"/>
+      <c r="Y6" s="124"/>
+      <c r="Z6" s="122"/>
+      <c r="AA6" s="123"/>
+      <c r="AB6" s="123"/>
+      <c r="AC6" s="124"/>
+    </row>
+    <row r="7" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A7" s="78" t="s">
+        <v>70</v>
+      </c>
+      <c r="B7" s="74">
+        <v>13</v>
+      </c>
+      <c r="C7" s="72">
+        <v>152.4</v>
+      </c>
+      <c r="D7" s="72"/>
+      <c r="E7" s="73">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F7" s="83">
+        <v>7</v>
+      </c>
+      <c r="G7" s="84"/>
+      <c r="H7" s="84"/>
+      <c r="I7" s="85"/>
+      <c r="J7" s="65"/>
+      <c r="K7" s="66">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+      <c r="L7" s="66" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M7" s="153">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N7" s="154">
+        <v>15</v>
+      </c>
+      <c r="O7" s="155"/>
+      <c r="P7" s="155"/>
+      <c r="Q7" s="156"/>
+      <c r="R7" s="157"/>
+      <c r="S7" s="158">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="T7" s="158" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U7" s="167">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="V7" s="122"/>
+      <c r="W7" s="123"/>
+      <c r="X7" s="123"/>
+      <c r="Y7" s="124"/>
+      <c r="Z7" s="122"/>
+      <c r="AA7" s="123"/>
+      <c r="AB7" s="123"/>
+      <c r="AC7" s="124"/>
+    </row>
+    <row r="8" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="78" t="s">
+        <v>71</v>
+      </c>
+      <c r="B8" s="80">
+        <v>19</v>
+      </c>
+      <c r="C8" s="81">
+        <v>152.4</v>
+      </c>
+      <c r="D8" s="81"/>
+      <c r="E8" s="82">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F8" s="67">
+        <v>13</v>
+      </c>
+      <c r="G8" s="68"/>
+      <c r="H8" s="68"/>
+      <c r="I8" s="69"/>
+      <c r="J8" s="70"/>
+      <c r="K8" s="89">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+      <c r="L8" s="89" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M8" s="168">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N8" s="166">
+        <v>16</v>
+      </c>
+      <c r="O8" s="167"/>
+      <c r="P8" s="167"/>
+      <c r="Q8" s="169"/>
+      <c r="R8" s="170"/>
+      <c r="S8" s="171">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="T8" s="171" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U8" s="171">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="V8" s="122"/>
+      <c r="W8" s="123"/>
+      <c r="X8" s="123"/>
+      <c r="Y8" s="124"/>
+      <c r="Z8" s="122"/>
+      <c r="AA8" s="123"/>
+      <c r="AB8" s="123"/>
+      <c r="AC8" s="124"/>
+    </row>
+    <row r="9" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A9" s="78" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="74">
+        <v>15</v>
+      </c>
+      <c r="C9" s="75">
+        <v>152.4</v>
+      </c>
+      <c r="D9" s="75"/>
+      <c r="E9" s="76">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F9" s="86"/>
+      <c r="G9" s="87"/>
+      <c r="H9" s="87"/>
+      <c r="I9" s="88"/>
+      <c r="J9" s="67"/>
+      <c r="K9" s="68">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+      <c r="L9" s="68" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M9" s="69">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N9" s="145"/>
+      <c r="O9" s="164"/>
+      <c r="P9" s="164"/>
+      <c r="Q9" s="165"/>
+      <c r="R9" s="166"/>
+      <c r="S9" s="167">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="T9" s="167" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U9" s="167">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="V9" s="122"/>
+      <c r="W9" s="123"/>
+      <c r="X9" s="123"/>
+      <c r="Y9" s="124"/>
+      <c r="Z9" s="122"/>
+      <c r="AA9" s="123"/>
+      <c r="AB9" s="123"/>
+      <c r="AC9" s="124"/>
+    </row>
+    <row r="10" spans="1:29" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" s="80">
+        <v>19</v>
+      </c>
+      <c r="C10" s="81">
+        <v>152.4</v>
+      </c>
+      <c r="D10" s="81"/>
+      <c r="E10" s="82">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F10" s="67"/>
+      <c r="G10" s="68"/>
+      <c r="H10" s="68"/>
+      <c r="I10" s="69"/>
+      <c r="J10" s="70"/>
+      <c r="K10" s="89">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+      <c r="L10" s="89" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M10" s="168">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N10" s="166"/>
+      <c r="O10" s="167"/>
+      <c r="P10" s="167"/>
+      <c r="Q10" s="169"/>
+      <c r="R10" s="170"/>
+      <c r="S10" s="171">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="T10" s="171" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U10" s="171">
+        <f t="shared" si="1"/>
+        <v>-1</v>
+      </c>
+      <c r="V10" s="122"/>
+      <c r="W10" s="123"/>
+      <c r="X10" s="123"/>
+      <c r="Y10" s="124"/>
+      <c r="Z10" s="122"/>
+      <c r="AA10" s="123"/>
+      <c r="AB10" s="123"/>
+      <c r="AC10" s="124"/>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A11" s="78" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="177">
+        <v>123</v>
+      </c>
+      <c r="C11" s="178">
+        <v>152.4</v>
+      </c>
+      <c r="D11" s="178"/>
+      <c r="E11" s="179">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F11" s="184">
+        <v>123456</v>
+      </c>
+      <c r="G11" s="185"/>
+      <c r="H11" s="185"/>
+      <c r="I11" s="186"/>
+      <c r="J11" s="141"/>
+      <c r="K11" s="142">
+        <f t="shared" si="2"/>
+        <v>-100</v>
+      </c>
+      <c r="L11" s="142" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M11" s="143">
+        <f t="shared" si="0"/>
+        <v>-100</v>
+      </c>
+      <c r="N11" s="191" t="s">
+        <v>60</v>
+      </c>
+      <c r="O11" s="191" t="s">
+        <v>60</v>
+      </c>
+      <c r="P11" s="191" t="s">
+        <v>60</v>
+      </c>
+      <c r="Q11" s="191" t="s">
+        <v>60</v>
+      </c>
+      <c r="R11" s="172" t="s">
+        <v>60</v>
+      </c>
+      <c r="S11" s="172" t="s">
+        <v>60</v>
+      </c>
+      <c r="T11" s="172" t="s">
+        <v>60</v>
+      </c>
+      <c r="U11" s="172" t="s">
+        <v>60</v>
+      </c>
+      <c r="V11" s="147"/>
+      <c r="W11" s="148"/>
+      <c r="X11" s="148"/>
+      <c r="Y11" s="149"/>
+      <c r="Z11" s="147"/>
+      <c r="AA11" s="148"/>
+      <c r="AB11" s="148"/>
+      <c r="AC11" s="149"/>
+    </row>
+    <row r="12" spans="1:29" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="79" t="s">
+        <v>53</v>
+      </c>
+      <c r="B12" s="180">
+        <v>8</v>
+      </c>
+      <c r="C12" s="181">
+        <v>152.4</v>
+      </c>
+      <c r="D12" s="181"/>
+      <c r="E12" s="182">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="F12" s="183">
+        <v>12</v>
+      </c>
+      <c r="G12" s="173">
+        <v>167.1</v>
+      </c>
+      <c r="H12" s="173"/>
+      <c r="I12" s="174">
+        <v>7.5350000000000001</v>
+      </c>
+      <c r="J12" s="187">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="188">
+        <f t="shared" si="2"/>
+        <v>9.6456692913385744</v>
+      </c>
+      <c r="L12" s="189" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M12" s="190">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N12" s="192">
+        <v>10</v>
+      </c>
+      <c r="O12" s="175"/>
+      <c r="P12" s="175"/>
+      <c r="Q12" s="176"/>
+      <c r="R12" s="193">
+        <v>0.25</v>
+      </c>
+      <c r="S12" s="194">
+        <f t="shared" si="3"/>
+        <v>-1</v>
+      </c>
+      <c r="T12" s="194" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U12" s="195">
+        <f>(Q12-E12)/E12</f>
+        <v>-1</v>
+      </c>
+      <c r="V12" s="150" t="s">
+        <v>75</v>
+      </c>
+      <c r="W12" s="151"/>
+      <c r="X12" s="151"/>
+      <c r="Y12" s="152"/>
+      <c r="Z12" s="150"/>
+      <c r="AA12" s="151"/>
+      <c r="AB12" s="151"/>
+      <c r="AC12" s="152"/>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A13" s="58"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="58"/>
+      <c r="E13" s="58"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="58"/>
+      <c r="I13" s="58"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="58"/>
+      <c r="L13" s="58"/>
+      <c r="M13" s="58"/>
+    </row>
+    <row r="14" spans="1:29" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="H14" s="146" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.3">
+      <c r="A16" s="61" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="120" t="s">
+        <v>54</v>
+      </c>
+      <c r="C16" s="120"/>
+      <c r="D16" s="121"/>
+      <c r="H16" s="62" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" s="59" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17" s="116" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="116"/>
+      <c r="D17" s="117"/>
+      <c r="G17" s="63" t="s">
+        <v>60</v>
+      </c>
+      <c r="H17" s="64" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="118" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="118"/>
+      <c r="D18" s="119"/>
+      <c r="F18" t="s">
+        <v>58</v>
+      </c>
+      <c r="G18" s="144" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="29">
+    <mergeCell ref="Z12:AC12"/>
+    <mergeCell ref="Z6:AC6"/>
+    <mergeCell ref="Z7:AC7"/>
+    <mergeCell ref="Z8:AC8"/>
+    <mergeCell ref="Z9:AC9"/>
+    <mergeCell ref="Z10:AC10"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="Z1:AC2"/>
+    <mergeCell ref="Z3:AC3"/>
+    <mergeCell ref="Z4:AC4"/>
+    <mergeCell ref="Z5:AC5"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="V1:Y2"/>
+    <mergeCell ref="V3:Y3"/>
+    <mergeCell ref="V4:Y4"/>
+    <mergeCell ref="V5:Y5"/>
+    <mergeCell ref="V6:Y6"/>
+    <mergeCell ref="V7:Y7"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="R1:U1"/>
+    <mergeCell ref="V8:Y8"/>
+    <mergeCell ref="V9:Y9"/>
+    <mergeCell ref="V10:Y10"/>
+    <mergeCell ref="V12:Y12"/>
+    <mergeCell ref="B17:D17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="c5ae091c-4d86-42b7-bd6d-05a6d5850206">
-      <UserInfo>
-        <DisplayName>Integrantes de la CURSO 1º MUSE</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2149,20 +4071,23 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="c5ae091c-4d86-42b7-bd6d-05a6d5850206">
+      <UserInfo>
+        <DisplayName>Integrantes de la CURSO 1º MUSE</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F2DDC3-8EF2-4F40-AEC5-CBD2E661EA55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A54CB81-BDC2-4F30-B8AA-8FF202FE488F}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5ae091c-4d86-42b7-bd6d-05a6d5850206"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2187,9 +4112,11 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A54CB81-BDC2-4F30-B8AA-8FF202FE488F}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F2DDC3-8EF2-4F40-AEC5-CBD2E661EA55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5ae091c-4d86-42b7-bd6d-05a6d5850206"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
++optimizacion, ahora forma en T
</commit_message>
<xml_diff>
--- a/MicroSat/Iteraciones.xlsx
+++ b/MicroSat/Iteraciones.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\MEng Space Systems (Local)\2. EUE\Micro-Satellite Design &amp; Analysis\MicroSat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10586D4F-BBC7-4F40-BF46-4E23DC95055B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FDE94F7-748E-4252-8D9D-167ADB97D3B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="121">
   <si>
     <t>Nº rigidizadores</t>
   </si>
@@ -396,6 +396,12 @@
   </si>
   <si>
     <t>Sat_Bandeja_Inf_9rig_T_Al7075_OPTIMIZACION_SOL1</t>
+  </si>
+  <si>
+    <t>Sat_Bandeja_Inf_9rig_T_Al7075_OPTIMIZACION_SOL2   (MISMA LONG RIG)</t>
+  </si>
+  <si>
+    <t>Sat_Bandeja_Inf_9rig_T_Al7075_OPTIMIZACION_SOL3 (MISMA LONG RIG)</t>
   </si>
 </sst>
 </file>
@@ -4187,8 +4193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA3D57E-AF43-4403-B1EC-4764DD27CECF}">
   <dimension ref="A2:Y86"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:L18"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="N53" sqref="N53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6513,14 +6519,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7277F0-43A1-4A40-97D9-A023F961F6A8}">
-  <dimension ref="A2:L17"/>
+  <dimension ref="A2:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="15.6640625" customWidth="1"/>
     <col min="10" max="10" width="2.5546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6910,11 +6917,789 @@
         <v>4.9280956864386081</v>
       </c>
     </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" s="198" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" s="203" t="s">
+        <v>88</v>
+      </c>
+      <c r="B21" s="204"/>
+      <c r="C21" s="204"/>
+      <c r="D21" s="204"/>
+      <c r="E21" s="204"/>
+      <c r="F21" s="204"/>
+      <c r="G21" s="204"/>
+      <c r="H21" s="204"/>
+      <c r="I21" s="204"/>
+      <c r="J21" s="204"/>
+      <c r="K21" s="204"/>
+      <c r="L21" s="205"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" s="192" t="s">
+        <v>89</v>
+      </c>
+      <c r="B22" s="196"/>
+      <c r="C22" s="188" t="s">
+        <v>90</v>
+      </c>
+      <c r="D22" s="188" t="s">
+        <v>91</v>
+      </c>
+      <c r="E22" s="188" t="s">
+        <v>92</v>
+      </c>
+      <c r="F22" s="188" t="s">
+        <v>93</v>
+      </c>
+      <c r="G22" s="188" t="s">
+        <v>94</v>
+      </c>
+      <c r="H22" s="188" t="s">
+        <v>95</v>
+      </c>
+      <c r="I22" s="188" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="188"/>
+      <c r="K22" s="188" t="s">
+        <v>97</v>
+      </c>
+      <c r="L22" s="189" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="193">
+        <v>85000000</v>
+      </c>
+      <c r="B23" s="197" t="s">
+        <v>102</v>
+      </c>
+      <c r="C23" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D23" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E23" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F23" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G23" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H23" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I23" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J23" s="190"/>
+      <c r="K23" s="194">
+        <f>(H23/(A23*C23*D23*E23*F23))-1</f>
+        <v>2.1967708195223987</v>
+      </c>
+      <c r="L23" s="195">
+        <f>(I23/(A23*C23*D23*E23*G23))-1</f>
+        <v>2.3057851239669414</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="193">
+        <v>52800000</v>
+      </c>
+      <c r="B24" s="197" t="s">
+        <v>103</v>
+      </c>
+      <c r="C24" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D24" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E24" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F24" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G24" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H24" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I24" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J24" s="190"/>
+      <c r="K24" s="194">
+        <f>(H24/(A24*C24*D24*E24*F24))-1</f>
+        <v>4.1463166602159838</v>
+      </c>
+      <c r="L24" s="195">
+        <f>(I24/(A24*C24*D24*E24*G24))-1</f>
+        <v>4.3218131730528428</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" s="203" t="s">
+        <v>101</v>
+      </c>
+      <c r="B26" s="204"/>
+      <c r="C26" s="204"/>
+      <c r="D26" s="204"/>
+      <c r="E26" s="204"/>
+      <c r="F26" s="204"/>
+      <c r="G26" s="204"/>
+      <c r="H26" s="204"/>
+      <c r="I26" s="204"/>
+      <c r="J26" s="204"/>
+      <c r="K26" s="204"/>
+      <c r="L26" s="205"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" s="192" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="196"/>
+      <c r="C27" s="188" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="188" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="188" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="188" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="188" t="s">
+        <v>94</v>
+      </c>
+      <c r="H27" s="188" t="s">
+        <v>95</v>
+      </c>
+      <c r="I27" s="188" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="188"/>
+      <c r="K27" s="188" t="s">
+        <v>97</v>
+      </c>
+      <c r="L27" s="189" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="193">
+        <v>79600000</v>
+      </c>
+      <c r="B28" s="197" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D28" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E28" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F28" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G28" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H28" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I28" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J28" s="190"/>
+      <c r="K28" s="194">
+        <f>(H28/(A28*C28*D28*E28*F28))-1</f>
+        <v>2.4136371816508029</v>
+      </c>
+      <c r="L28" s="194">
+        <f>(I28/(A28*C28*D28*E28*G28))-1</f>
+        <v>2.5300469288591714</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="193">
+        <v>61400000</v>
+      </c>
+      <c r="B29" s="197" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D29" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E29" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F29" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G29" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H29" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I29" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J29" s="190"/>
+      <c r="K29" s="194">
+        <f>(H29/(A29*C29*D29*E29*F29))-1</f>
+        <v>3.4254970628567412</v>
+      </c>
+      <c r="L29" s="194">
+        <f>(I29/(A29*C29*D29*E29*G29))-1</f>
+        <v>3.5764126308988615</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" s="203" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="204"/>
+      <c r="C31" s="204"/>
+      <c r="D31" s="204"/>
+      <c r="E31" s="204"/>
+      <c r="F31" s="204"/>
+      <c r="G31" s="204"/>
+      <c r="H31" s="204"/>
+      <c r="I31" s="204"/>
+      <c r="J31" s="204"/>
+      <c r="K31" s="204"/>
+      <c r="L31" s="205"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" s="192" t="s">
+        <v>99</v>
+      </c>
+      <c r="B32" s="196"/>
+      <c r="C32" s="188" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="188" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="188" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="188" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="188" t="s">
+        <v>94</v>
+      </c>
+      <c r="H32" s="188" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" s="188" t="s">
+        <v>96</v>
+      </c>
+      <c r="J32" s="188"/>
+      <c r="K32" s="188" t="s">
+        <v>97</v>
+      </c>
+      <c r="L32" s="189" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="193">
+        <v>79600000</v>
+      </c>
+      <c r="B33" s="197" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D33" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E33" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F33" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G33" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H33" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I33" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J33" s="190"/>
+      <c r="K33" s="194">
+        <f>(H33/(A33*C33*D33*E33*F33))-1</f>
+        <v>2.4136371816508029</v>
+      </c>
+      <c r="L33" s="195">
+        <f>(I33/(A33*C33*D33*E33*G33))-1</f>
+        <v>2.5300469288591714</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="193">
+        <v>46700000</v>
+      </c>
+      <c r="B34" s="197" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D34" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E34" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F34" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G34" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H34" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I34" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J34" s="190"/>
+      <c r="K34" s="194">
+        <f>(H34/(A34*C34*D34*E34*F34))-1</f>
+        <v>4.8185336115504036</v>
+      </c>
+      <c r="L34" s="195">
+        <f>(I34/(A34*C34*D34*E34*G34))-1</f>
+        <v>5.016953651759958</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="198" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A38" s="203" t="s">
+        <v>88</v>
+      </c>
+      <c r="B38" s="204"/>
+      <c r="C38" s="204"/>
+      <c r="D38" s="204"/>
+      <c r="E38" s="204"/>
+      <c r="F38" s="204"/>
+      <c r="G38" s="204"/>
+      <c r="H38" s="204"/>
+      <c r="I38" s="204"/>
+      <c r="J38" s="204"/>
+      <c r="K38" s="204"/>
+      <c r="L38" s="205"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A39" s="192" t="s">
+        <v>89</v>
+      </c>
+      <c r="B39" s="196"/>
+      <c r="C39" s="188" t="s">
+        <v>90</v>
+      </c>
+      <c r="D39" s="188" t="s">
+        <v>91</v>
+      </c>
+      <c r="E39" s="188" t="s">
+        <v>92</v>
+      </c>
+      <c r="F39" s="188" t="s">
+        <v>93</v>
+      </c>
+      <c r="G39" s="188" t="s">
+        <v>94</v>
+      </c>
+      <c r="H39" s="188" t="s">
+        <v>95</v>
+      </c>
+      <c r="I39" s="188" t="s">
+        <v>96</v>
+      </c>
+      <c r="J39" s="188"/>
+      <c r="K39" s="188" t="s">
+        <v>97</v>
+      </c>
+      <c r="L39" s="189" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="193">
+        <v>85600000</v>
+      </c>
+      <c r="B40" s="197" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D40" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E40" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F40" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G40" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H40" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I40" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J40" s="190"/>
+      <c r="K40" s="194">
+        <f>(H40/(A40*C40*D40*E40*F40))-1</f>
+        <v>2.1743635474229426</v>
+      </c>
+      <c r="L40" s="195">
+        <f>(I40/(A40*C40*D40*E40*G40))-1</f>
+        <v>2.2826137329110985</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="193">
+        <v>43000000</v>
+      </c>
+      <c r="B41" s="197" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D41" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E41" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F41" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G41" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H41" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I41" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J41" s="190"/>
+      <c r="K41" s="194">
+        <f>(H41/(A41*C41*D41*E41*F41))-1</f>
+        <v>5.3191981316140442</v>
+      </c>
+      <c r="L41" s="195">
+        <f>(I41/(A41*C41*D41*E41*G41))-1</f>
+        <v>5.5346915241206984</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="203" t="s">
+        <v>101</v>
+      </c>
+      <c r="B43" s="204"/>
+      <c r="C43" s="204"/>
+      <c r="D43" s="204"/>
+      <c r="E43" s="204"/>
+      <c r="F43" s="204"/>
+      <c r="G43" s="204"/>
+      <c r="H43" s="204"/>
+      <c r="I43" s="204"/>
+      <c r="J43" s="204"/>
+      <c r="K43" s="204"/>
+      <c r="L43" s="205"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="192" t="s">
+        <v>100</v>
+      </c>
+      <c r="B44" s="196"/>
+      <c r="C44" s="188" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="188" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="188" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="188" t="s">
+        <v>93</v>
+      </c>
+      <c r="G44" s="188" t="s">
+        <v>94</v>
+      </c>
+      <c r="H44" s="188" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" s="188" t="s">
+        <v>96</v>
+      </c>
+      <c r="J44" s="188"/>
+      <c r="K44" s="188" t="s">
+        <v>97</v>
+      </c>
+      <c r="L44" s="189" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="193">
+        <v>83500000</v>
+      </c>
+      <c r="B45" s="197" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D45" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E45" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F45" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G45" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H45" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I45" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J45" s="190"/>
+      <c r="K45" s="194">
+        <f>(H45/(A45*C45*D45*E45*F45))-1</f>
+        <v>2.2541978402323819</v>
+      </c>
+      <c r="L45" s="194">
+        <f>(I45/(A45*C45*D45*E45*G45))-1</f>
+        <v>2.3651704854753297</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="193">
+        <v>64400000</v>
+      </c>
+      <c r="B46" s="197" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D46" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E46" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F46" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G46" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H46" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I46" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J46" s="190"/>
+      <c r="K46" s="194">
+        <f>(H46/(A46*C46*D46*E46*F46))-1</f>
+        <v>3.2193403673820482</v>
+      </c>
+      <c r="L46" s="194">
+        <f>(I46/(A46*C46*D46*E46*G46))-1</f>
+        <v>3.3632257070992244</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="203" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="204"/>
+      <c r="C48" s="204"/>
+      <c r="D48" s="204"/>
+      <c r="E48" s="204"/>
+      <c r="F48" s="204"/>
+      <c r="G48" s="204"/>
+      <c r="H48" s="204"/>
+      <c r="I48" s="204"/>
+      <c r="J48" s="204"/>
+      <c r="K48" s="204"/>
+      <c r="L48" s="205"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="192" t="s">
+        <v>99</v>
+      </c>
+      <c r="B49" s="196"/>
+      <c r="C49" s="188" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="188" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="188" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="188" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" s="188" t="s">
+        <v>94</v>
+      </c>
+      <c r="H49" s="188" t="s">
+        <v>95</v>
+      </c>
+      <c r="I49" s="188" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" s="188"/>
+      <c r="K49" s="188" t="s">
+        <v>97</v>
+      </c>
+      <c r="L49" s="189" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="193">
+        <v>83500000</v>
+      </c>
+      <c r="B50" s="197" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D50" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E50" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F50" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G50" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H50" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I50" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J50" s="190"/>
+      <c r="K50" s="194">
+        <f>(H50/(A50*C50*D50*E50*F50))-1</f>
+        <v>2.2541978402323819</v>
+      </c>
+      <c r="L50" s="195">
+        <f>(I50/(A50*C50*D50*E50*G50))-1</f>
+        <v>2.3651704854753297</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="193">
+        <v>44200000</v>
+      </c>
+      <c r="B51" s="197" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D51" s="190">
+        <v>1.2</v>
+      </c>
+      <c r="E51" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F51" s="190">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G51" s="190">
+        <v>1.25</v>
+      </c>
+      <c r="H51" s="191">
+        <v>434000000</v>
+      </c>
+      <c r="I51" s="191">
+        <v>510000000</v>
+      </c>
+      <c r="J51" s="190"/>
+      <c r="K51" s="194">
+        <f>(H51/(A51*C51*D51*E51*F51))-1</f>
+        <v>5.1476361913892283</v>
+      </c>
+      <c r="L51" s="195">
+        <f>(I51/(A51*C51*D51*E51*G51))-1</f>
+        <v>5.357279084551811</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A48:L48"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A21:L21"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6924,7 +7709,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C65A9CD-A62A-4089-A8C2-03B1AF135CF1}">
   <dimension ref="A2:L53"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Sol secc T con sentido
</commit_message>
<xml_diff>
--- a/MicroSat/Iteraciones.xlsx
+++ b/MicroSat/Iteraciones.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\MEng Space Systems (Local)\2. EUE\Micro-Satellite Design &amp; Analysis\MicroSat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92772112-DB6F-491E-B151-1B05699F4D82}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0173F7D7-0598-4FDE-AE34-E539F53D8C84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="It_Bandeja Inf" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="804" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="122">
   <si>
     <t>Nº rigidizadores</t>
   </si>
@@ -402,6 +402,9 @@
   </si>
   <si>
     <t>Sat_Bandeja_Inf_9rig_T_Al7075_OPTIMIZACION_SOL3 (MISMA LONG RIG)</t>
+  </si>
+  <si>
+    <t>Sat_Bandeja_Inf_9rig_T_Al7075_OPTIMIZACION_SOL4 (MISMA LONG RIG)</t>
   </si>
 </sst>
 </file>
@@ -1794,178 +1797,178 @@
     <xf numFmtId="0" fontId="9" fillId="19" borderId="0" xfId="18" applyFont="1"/>
     <xf numFmtId="11" fontId="1" fillId="18" borderId="0" xfId="17" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="2" fillId="3" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="21" borderId="42" xfId="20"/>
     <xf numFmtId="0" fontId="10" fillId="20" borderId="17" xfId="19" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="45" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="46" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="46" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="46" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="46" xfId="16" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="47" xfId="15" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="33" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="27" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="5" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="25" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="8" borderId="5" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="7" borderId="22" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="18" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="48" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="13" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="43" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="44" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="13" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="49" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="16" xfId="19" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="20" borderId="18" xfId="19" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="20" borderId="19" xfId="19" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="14" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="16" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="43" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="44" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="45" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="46" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="46" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="46" xfId="14" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="46" xfId="16" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="47" xfId="15" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="1" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="2" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="3" xfId="8" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="33" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="8" borderId="27" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="5" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="25" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="8" borderId="5" xfId="7" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="7" borderId="22" xfId="6" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="18" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="48" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="13" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="49" xfId="19" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="13" xfId="19" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="15" xfId="19" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="1" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="2" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="1" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="2" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="3" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="21">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -3862,20 +3865,20 @@
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="194"/>
-      <c r="C4" s="194"/>
-      <c r="D4" s="194"/>
-      <c r="E4" s="194"/>
-      <c r="F4" s="194"/>
-      <c r="G4" s="194"/>
-      <c r="H4" s="194"/>
-      <c r="I4" s="194"/>
-      <c r="J4" s="194"/>
-      <c r="K4" s="194"/>
-      <c r="L4" s="195"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
+      <c r="H4" s="213"/>
+      <c r="I4" s="213"/>
+      <c r="J4" s="213"/>
+      <c r="K4" s="213"/>
+      <c r="L4" s="214"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="182" t="s">
@@ -3989,20 +3992,20 @@
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="194"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="195"/>
+      <c r="B9" s="213"/>
+      <c r="C9" s="213"/>
+      <c r="D9" s="213"/>
+      <c r="E9" s="213"/>
+      <c r="F9" s="213"/>
+      <c r="G9" s="213"/>
+      <c r="H9" s="213"/>
+      <c r="I9" s="213"/>
+      <c r="J9" s="213"/>
+      <c r="K9" s="213"/>
+      <c r="L9" s="214"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="182" t="s">
@@ -4116,20 +4119,20 @@
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="193" t="s">
+      <c r="A14" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="194"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="194"/>
-      <c r="E14" s="194"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="194"/>
-      <c r="H14" s="194"/>
-      <c r="I14" s="194"/>
-      <c r="J14" s="194"/>
-      <c r="K14" s="194"/>
-      <c r="L14" s="195"/>
+      <c r="B14" s="213"/>
+      <c r="C14" s="213"/>
+      <c r="D14" s="213"/>
+      <c r="E14" s="213"/>
+      <c r="F14" s="213"/>
+      <c r="G14" s="213"/>
+      <c r="H14" s="213"/>
+      <c r="I14" s="213"/>
+      <c r="J14" s="213"/>
+      <c r="K14" s="213"/>
+      <c r="L14" s="214"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="182" t="s">
@@ -4327,37 +4330,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="225" t="s">
+      <c r="A2" s="193" t="s">
         <v>111</v>
       </c>
-      <c r="B2" s="225"/>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225"/>
-      <c r="I2" s="225"/>
-      <c r="J2" s="225"/>
-      <c r="K2" s="225"/>
-      <c r="L2" s="225"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="194"/>
-      <c r="C4" s="194"/>
-      <c r="D4" s="194"/>
-      <c r="E4" s="194"/>
-      <c r="F4" s="194"/>
-      <c r="G4" s="194"/>
-      <c r="H4" s="194"/>
-      <c r="I4" s="194"/>
-      <c r="J4" s="194"/>
-      <c r="K4" s="194"/>
-      <c r="L4" s="195"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
+      <c r="H4" s="213"/>
+      <c r="I4" s="213"/>
+      <c r="J4" s="213"/>
+      <c r="K4" s="213"/>
+      <c r="L4" s="214"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="182" t="s">
@@ -4471,20 +4474,20 @@
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="194"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="195"/>
+      <c r="B9" s="213"/>
+      <c r="C9" s="213"/>
+      <c r="D9" s="213"/>
+      <c r="E9" s="213"/>
+      <c r="F9" s="213"/>
+      <c r="G9" s="213"/>
+      <c r="H9" s="213"/>
+      <c r="I9" s="213"/>
+      <c r="J9" s="213"/>
+      <c r="K9" s="213"/>
+      <c r="L9" s="214"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="182" t="s">
@@ -4598,20 +4601,20 @@
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="193" t="s">
+      <c r="A14" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="194"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="194"/>
-      <c r="E14" s="194"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="194"/>
-      <c r="H14" s="194"/>
-      <c r="I14" s="194"/>
-      <c r="J14" s="194"/>
-      <c r="K14" s="194"/>
-      <c r="L14" s="195"/>
+      <c r="B14" s="213"/>
+      <c r="C14" s="213"/>
+      <c r="D14" s="213"/>
+      <c r="E14" s="213"/>
+      <c r="F14" s="213"/>
+      <c r="G14" s="213"/>
+      <c r="H14" s="213"/>
+      <c r="I14" s="213"/>
+      <c r="J14" s="213"/>
+      <c r="K14" s="213"/>
+      <c r="L14" s="214"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="182" t="s">
@@ -4724,37 +4727,37 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="225" t="s">
+      <c r="A19" s="193" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="225"/>
-      <c r="C19" s="225"/>
-      <c r="D19" s="225"/>
-      <c r="E19" s="225"/>
-      <c r="F19" s="225"/>
-      <c r="G19" s="225"/>
-      <c r="H19" s="225"/>
-      <c r="I19" s="225"/>
-      <c r="J19" s="225"/>
-      <c r="K19" s="225"/>
-      <c r="L19" s="225"/>
+      <c r="B19" s="193"/>
+      <c r="C19" s="193"/>
+      <c r="D19" s="193"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
+      <c r="K19" s="193"/>
+      <c r="L19" s="193"/>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="193" t="s">
+      <c r="A21" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="194"/>
-      <c r="C21" s="194"/>
-      <c r="D21" s="194"/>
-      <c r="E21" s="194"/>
-      <c r="F21" s="194"/>
-      <c r="G21" s="194"/>
-      <c r="H21" s="194"/>
-      <c r="I21" s="194"/>
-      <c r="J21" s="194"/>
-      <c r="K21" s="194"/>
-      <c r="L21" s="195"/>
+      <c r="B21" s="213"/>
+      <c r="C21" s="213"/>
+      <c r="D21" s="213"/>
+      <c r="E21" s="213"/>
+      <c r="F21" s="213"/>
+      <c r="G21" s="213"/>
+      <c r="H21" s="213"/>
+      <c r="I21" s="213"/>
+      <c r="J21" s="213"/>
+      <c r="K21" s="213"/>
+      <c r="L21" s="214"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="182" t="s">
@@ -4868,20 +4871,20 @@
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="193" t="s">
+      <c r="A26" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="194"/>
-      <c r="C26" s="194"/>
-      <c r="D26" s="194"/>
-      <c r="E26" s="194"/>
-      <c r="F26" s="194"/>
-      <c r="G26" s="194"/>
-      <c r="H26" s="194"/>
-      <c r="I26" s="194"/>
-      <c r="J26" s="194"/>
-      <c r="K26" s="194"/>
-      <c r="L26" s="195"/>
+      <c r="B26" s="213"/>
+      <c r="C26" s="213"/>
+      <c r="D26" s="213"/>
+      <c r="E26" s="213"/>
+      <c r="F26" s="213"/>
+      <c r="G26" s="213"/>
+      <c r="H26" s="213"/>
+      <c r="I26" s="213"/>
+      <c r="J26" s="213"/>
+      <c r="K26" s="213"/>
+      <c r="L26" s="214"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="182" t="s">
@@ -4995,20 +4998,20 @@
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="193" t="s">
+      <c r="A31" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="194"/>
-      <c r="C31" s="194"/>
-      <c r="D31" s="194"/>
-      <c r="E31" s="194"/>
-      <c r="F31" s="194"/>
-      <c r="G31" s="194"/>
-      <c r="H31" s="194"/>
-      <c r="I31" s="194"/>
-      <c r="J31" s="194"/>
-      <c r="K31" s="194"/>
-      <c r="L31" s="195"/>
+      <c r="B31" s="213"/>
+      <c r="C31" s="213"/>
+      <c r="D31" s="213"/>
+      <c r="E31" s="213"/>
+      <c r="F31" s="213"/>
+      <c r="G31" s="213"/>
+      <c r="H31" s="213"/>
+      <c r="I31" s="213"/>
+      <c r="J31" s="213"/>
+      <c r="K31" s="213"/>
+      <c r="L31" s="214"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="182" t="s">
@@ -5121,37 +5124,37 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="225" t="s">
+      <c r="A36" s="193" t="s">
         <v>110</v>
       </c>
-      <c r="B36" s="225"/>
-      <c r="C36" s="225"/>
-      <c r="D36" s="225"/>
-      <c r="E36" s="225"/>
-      <c r="F36" s="225"/>
-      <c r="G36" s="225"/>
-      <c r="H36" s="225"/>
-      <c r="I36" s="225"/>
-      <c r="J36" s="225"/>
-      <c r="K36" s="225"/>
-      <c r="L36" s="225"/>
+      <c r="B36" s="193"/>
+      <c r="C36" s="193"/>
+      <c r="D36" s="193"/>
+      <c r="E36" s="193"/>
+      <c r="F36" s="193"/>
+      <c r="G36" s="193"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="193"/>
+      <c r="K36" s="193"/>
+      <c r="L36" s="193"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="193" t="s">
+      <c r="A38" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="194"/>
-      <c r="C38" s="194"/>
-      <c r="D38" s="194"/>
-      <c r="E38" s="194"/>
-      <c r="F38" s="194"/>
-      <c r="G38" s="194"/>
-      <c r="H38" s="194"/>
-      <c r="I38" s="194"/>
-      <c r="J38" s="194"/>
-      <c r="K38" s="194"/>
-      <c r="L38" s="195"/>
+      <c r="B38" s="213"/>
+      <c r="C38" s="213"/>
+      <c r="D38" s="213"/>
+      <c r="E38" s="213"/>
+      <c r="F38" s="213"/>
+      <c r="G38" s="213"/>
+      <c r="H38" s="213"/>
+      <c r="I38" s="213"/>
+      <c r="J38" s="213"/>
+      <c r="K38" s="213"/>
+      <c r="L38" s="214"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="182" t="s">
@@ -5265,20 +5268,20 @@
     </row>
     <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="193" t="s">
+      <c r="A43" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="194"/>
-      <c r="C43" s="194"/>
-      <c r="D43" s="194"/>
-      <c r="E43" s="194"/>
-      <c r="F43" s="194"/>
-      <c r="G43" s="194"/>
-      <c r="H43" s="194"/>
-      <c r="I43" s="194"/>
-      <c r="J43" s="194"/>
-      <c r="K43" s="194"/>
-      <c r="L43" s="195"/>
+      <c r="B43" s="213"/>
+      <c r="C43" s="213"/>
+      <c r="D43" s="213"/>
+      <c r="E43" s="213"/>
+      <c r="F43" s="213"/>
+      <c r="G43" s="213"/>
+      <c r="H43" s="213"/>
+      <c r="I43" s="213"/>
+      <c r="J43" s="213"/>
+      <c r="K43" s="213"/>
+      <c r="L43" s="214"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="182" t="s">
@@ -5392,20 +5395,20 @@
     </row>
     <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="193" t="s">
+      <c r="A48" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="194"/>
-      <c r="C48" s="194"/>
-      <c r="D48" s="194"/>
-      <c r="E48" s="194"/>
-      <c r="F48" s="194"/>
-      <c r="G48" s="194"/>
-      <c r="H48" s="194"/>
-      <c r="I48" s="194"/>
-      <c r="J48" s="194"/>
-      <c r="K48" s="194"/>
-      <c r="L48" s="195"/>
+      <c r="B48" s="213"/>
+      <c r="C48" s="213"/>
+      <c r="D48" s="213"/>
+      <c r="E48" s="213"/>
+      <c r="F48" s="213"/>
+      <c r="G48" s="213"/>
+      <c r="H48" s="213"/>
+      <c r="I48" s="213"/>
+      <c r="J48" s="213"/>
+      <c r="K48" s="213"/>
+      <c r="L48" s="214"/>
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A49" s="182" t="s">
@@ -5518,65 +5521,65 @@
       </c>
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A53" s="225" t="s">
+      <c r="A53" s="193" t="s">
         <v>113</v>
       </c>
-      <c r="B53" s="225"/>
-      <c r="C53" s="225"/>
-      <c r="D53" s="225"/>
-      <c r="E53" s="225"/>
-      <c r="F53" s="225"/>
-      <c r="G53" s="225"/>
-      <c r="H53" s="225"/>
-      <c r="I53" s="225"/>
-      <c r="J53" s="225"/>
-      <c r="K53" s="225"/>
-      <c r="L53" s="225"/>
-      <c r="N53" s="225" t="s">
+      <c r="B53" s="193"/>
+      <c r="C53" s="193"/>
+      <c r="D53" s="193"/>
+      <c r="E53" s="193"/>
+      <c r="F53" s="193"/>
+      <c r="G53" s="193"/>
+      <c r="H53" s="193"/>
+      <c r="I53" s="193"/>
+      <c r="J53" s="193"/>
+      <c r="K53" s="193"/>
+      <c r="L53" s="193"/>
+      <c r="N53" s="193" t="s">
         <v>115</v>
       </c>
-      <c r="O53" s="225"/>
-      <c r="P53" s="225"/>
-      <c r="Q53" s="225"/>
-      <c r="R53" s="225"/>
-      <c r="S53" s="225"/>
-      <c r="T53" s="225"/>
-      <c r="U53" s="225"/>
-      <c r="V53" s="225"/>
-      <c r="W53" s="225"/>
-      <c r="X53" s="225"/>
-      <c r="Y53" s="225"/>
+      <c r="O53" s="193"/>
+      <c r="P53" s="193"/>
+      <c r="Q53" s="193"/>
+      <c r="R53" s="193"/>
+      <c r="S53" s="193"/>
+      <c r="T53" s="193"/>
+      <c r="U53" s="193"/>
+      <c r="V53" s="193"/>
+      <c r="W53" s="193"/>
+      <c r="X53" s="193"/>
+      <c r="Y53" s="193"/>
     </row>
     <row r="54" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="55" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A55" s="193" t="s">
+      <c r="A55" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B55" s="194"/>
-      <c r="C55" s="194"/>
-      <c r="D55" s="194"/>
-      <c r="E55" s="194"/>
-      <c r="F55" s="194"/>
-      <c r="G55" s="194"/>
-      <c r="H55" s="194"/>
-      <c r="I55" s="194"/>
-      <c r="J55" s="194"/>
-      <c r="K55" s="194"/>
-      <c r="L55" s="195"/>
-      <c r="N55" s="193" t="s">
+      <c r="B55" s="213"/>
+      <c r="C55" s="213"/>
+      <c r="D55" s="213"/>
+      <c r="E55" s="213"/>
+      <c r="F55" s="213"/>
+      <c r="G55" s="213"/>
+      <c r="H55" s="213"/>
+      <c r="I55" s="213"/>
+      <c r="J55" s="213"/>
+      <c r="K55" s="213"/>
+      <c r="L55" s="214"/>
+      <c r="N55" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="O55" s="194"/>
-      <c r="P55" s="194"/>
-      <c r="Q55" s="194"/>
-      <c r="R55" s="194"/>
-      <c r="S55" s="194"/>
-      <c r="T55" s="194"/>
-      <c r="U55" s="194"/>
-      <c r="V55" s="194"/>
-      <c r="W55" s="194"/>
-      <c r="X55" s="194"/>
-      <c r="Y55" s="195"/>
+      <c r="O55" s="213"/>
+      <c r="P55" s="213"/>
+      <c r="Q55" s="213"/>
+      <c r="R55" s="213"/>
+      <c r="S55" s="213"/>
+      <c r="T55" s="213"/>
+      <c r="U55" s="213"/>
+      <c r="V55" s="213"/>
+      <c r="W55" s="213"/>
+      <c r="X55" s="213"/>
+      <c r="Y55" s="214"/>
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A56" s="182" t="s">
@@ -5794,34 +5797,34 @@
     </row>
     <row r="59" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="60" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A60" s="193" t="s">
+      <c r="A60" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="194"/>
-      <c r="C60" s="194"/>
-      <c r="D60" s="194"/>
-      <c r="E60" s="194"/>
-      <c r="F60" s="194"/>
-      <c r="G60" s="194"/>
-      <c r="H60" s="194"/>
-      <c r="I60" s="194"/>
-      <c r="J60" s="194"/>
-      <c r="K60" s="194"/>
-      <c r="L60" s="195"/>
-      <c r="N60" s="193" t="s">
+      <c r="B60" s="213"/>
+      <c r="C60" s="213"/>
+      <c r="D60" s="213"/>
+      <c r="E60" s="213"/>
+      <c r="F60" s="213"/>
+      <c r="G60" s="213"/>
+      <c r="H60" s="213"/>
+      <c r="I60" s="213"/>
+      <c r="J60" s="213"/>
+      <c r="K60" s="213"/>
+      <c r="L60" s="214"/>
+      <c r="N60" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="O60" s="194"/>
-      <c r="P60" s="194"/>
-      <c r="Q60" s="194"/>
-      <c r="R60" s="194"/>
-      <c r="S60" s="194"/>
-      <c r="T60" s="194"/>
-      <c r="U60" s="194"/>
-      <c r="V60" s="194"/>
-      <c r="W60" s="194"/>
-      <c r="X60" s="194"/>
-      <c r="Y60" s="195"/>
+      <c r="O60" s="213"/>
+      <c r="P60" s="213"/>
+      <c r="Q60" s="213"/>
+      <c r="R60" s="213"/>
+      <c r="S60" s="213"/>
+      <c r="T60" s="213"/>
+      <c r="U60" s="213"/>
+      <c r="V60" s="213"/>
+      <c r="W60" s="213"/>
+      <c r="X60" s="213"/>
+      <c r="Y60" s="214"/>
     </row>
     <row r="61" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A61" s="182" t="s">
@@ -6039,34 +6042,34 @@
     </row>
     <row r="64" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="65" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A65" s="193" t="s">
+      <c r="A65" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B65" s="194"/>
-      <c r="C65" s="194"/>
-      <c r="D65" s="194"/>
-      <c r="E65" s="194"/>
-      <c r="F65" s="194"/>
-      <c r="G65" s="194"/>
-      <c r="H65" s="194"/>
-      <c r="I65" s="194"/>
-      <c r="J65" s="194"/>
-      <c r="K65" s="194"/>
-      <c r="L65" s="195"/>
-      <c r="N65" s="193" t="s">
+      <c r="B65" s="213"/>
+      <c r="C65" s="213"/>
+      <c r="D65" s="213"/>
+      <c r="E65" s="213"/>
+      <c r="F65" s="213"/>
+      <c r="G65" s="213"/>
+      <c r="H65" s="213"/>
+      <c r="I65" s="213"/>
+      <c r="J65" s="213"/>
+      <c r="K65" s="213"/>
+      <c r="L65" s="214"/>
+      <c r="N65" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="O65" s="194"/>
-      <c r="P65" s="194"/>
-      <c r="Q65" s="194"/>
-      <c r="R65" s="194"/>
-      <c r="S65" s="194"/>
-      <c r="T65" s="194"/>
-      <c r="U65" s="194"/>
-      <c r="V65" s="194"/>
-      <c r="W65" s="194"/>
-      <c r="X65" s="194"/>
-      <c r="Y65" s="195"/>
+      <c r="O65" s="213"/>
+      <c r="P65" s="213"/>
+      <c r="Q65" s="213"/>
+      <c r="R65" s="213"/>
+      <c r="S65" s="213"/>
+      <c r="T65" s="213"/>
+      <c r="U65" s="213"/>
+      <c r="V65" s="213"/>
+      <c r="W65" s="213"/>
+      <c r="X65" s="213"/>
+      <c r="Y65" s="214"/>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A66" s="182" t="s">
@@ -6283,37 +6286,37 @@
       </c>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A71" s="225" t="s">
+      <c r="A71" s="193" t="s">
         <v>114</v>
       </c>
-      <c r="B71" s="225"/>
-      <c r="C71" s="225"/>
-      <c r="D71" s="225"/>
-      <c r="E71" s="225"/>
-      <c r="F71" s="225"/>
-      <c r="G71" s="225"/>
-      <c r="H71" s="225"/>
-      <c r="I71" s="225"/>
-      <c r="J71" s="225"/>
-      <c r="K71" s="225"/>
-      <c r="L71" s="225"/>
+      <c r="B71" s="193"/>
+      <c r="C71" s="193"/>
+      <c r="D71" s="193"/>
+      <c r="E71" s="193"/>
+      <c r="F71" s="193"/>
+      <c r="G71" s="193"/>
+      <c r="H71" s="193"/>
+      <c r="I71" s="193"/>
+      <c r="J71" s="193"/>
+      <c r="K71" s="193"/>
+      <c r="L71" s="193"/>
     </row>
     <row r="72" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="73" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A73" s="193" t="s">
+      <c r="A73" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B73" s="194"/>
-      <c r="C73" s="194"/>
-      <c r="D73" s="194"/>
-      <c r="E73" s="194"/>
-      <c r="F73" s="194"/>
-      <c r="G73" s="194"/>
-      <c r="H73" s="194"/>
-      <c r="I73" s="194"/>
-      <c r="J73" s="194"/>
-      <c r="K73" s="194"/>
-      <c r="L73" s="195"/>
+      <c r="B73" s="213"/>
+      <c r="C73" s="213"/>
+      <c r="D73" s="213"/>
+      <c r="E73" s="213"/>
+      <c r="F73" s="213"/>
+      <c r="G73" s="213"/>
+      <c r="H73" s="213"/>
+      <c r="I73" s="213"/>
+      <c r="J73" s="213"/>
+      <c r="K73" s="213"/>
+      <c r="L73" s="214"/>
     </row>
     <row r="74" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A74" s="182" t="s">
@@ -6427,20 +6430,20 @@
     </row>
     <row r="77" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="78" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="A78" s="193" t="s">
+      <c r="A78" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B78" s="194"/>
-      <c r="C78" s="194"/>
-      <c r="D78" s="194"/>
-      <c r="E78" s="194"/>
-      <c r="F78" s="194"/>
-      <c r="G78" s="194"/>
-      <c r="H78" s="194"/>
-      <c r="I78" s="194"/>
-      <c r="J78" s="194"/>
-      <c r="K78" s="194"/>
-      <c r="L78" s="195"/>
+      <c r="B78" s="213"/>
+      <c r="C78" s="213"/>
+      <c r="D78" s="213"/>
+      <c r="E78" s="213"/>
+      <c r="F78" s="213"/>
+      <c r="G78" s="213"/>
+      <c r="H78" s="213"/>
+      <c r="I78" s="213"/>
+      <c r="J78" s="213"/>
+      <c r="K78" s="213"/>
+      <c r="L78" s="214"/>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A79" s="182" t="s">
@@ -6554,20 +6557,20 @@
     </row>
     <row r="82" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" s="193" t="s">
+      <c r="A83" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B83" s="194"/>
-      <c r="C83" s="194"/>
-      <c r="D83" s="194"/>
-      <c r="E83" s="194"/>
-      <c r="F83" s="194"/>
-      <c r="G83" s="194"/>
-      <c r="H83" s="194"/>
-      <c r="I83" s="194"/>
-      <c r="J83" s="194"/>
-      <c r="K83" s="194"/>
-      <c r="L83" s="195"/>
+      <c r="B83" s="213"/>
+      <c r="C83" s="213"/>
+      <c r="D83" s="213"/>
+      <c r="E83" s="213"/>
+      <c r="F83" s="213"/>
+      <c r="G83" s="213"/>
+      <c r="H83" s="213"/>
+      <c r="I83" s="213"/>
+      <c r="J83" s="213"/>
+      <c r="K83" s="213"/>
+      <c r="L83" s="214"/>
     </row>
     <row r="84" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A84" s="182" t="s">
@@ -6681,24 +6684,24 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="N60:Y60"/>
+    <mergeCell ref="N55:Y55"/>
+    <mergeCell ref="N65:Y65"/>
+    <mergeCell ref="A55:L55"/>
+    <mergeCell ref="A60:L60"/>
+    <mergeCell ref="A65:L65"/>
+    <mergeCell ref="A83:L83"/>
+    <mergeCell ref="A78:L78"/>
+    <mergeCell ref="A73:L73"/>
+    <mergeCell ref="A38:L38"/>
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A48:L48"/>
     <mergeCell ref="A14:L14"/>
     <mergeCell ref="A21:L21"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A31:L31"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A9:L9"/>
-    <mergeCell ref="A83:L83"/>
-    <mergeCell ref="A78:L78"/>
-    <mergeCell ref="A73:L73"/>
-    <mergeCell ref="A38:L38"/>
-    <mergeCell ref="A43:L43"/>
-    <mergeCell ref="A48:L48"/>
-    <mergeCell ref="N60:Y60"/>
-    <mergeCell ref="N55:Y55"/>
-    <mergeCell ref="N65:Y65"/>
-    <mergeCell ref="A55:L55"/>
-    <mergeCell ref="A60:L60"/>
-    <mergeCell ref="A65:L65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6706,10 +6709,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7277F0-43A1-4A40-97D9-A023F961F6A8}">
-  <dimension ref="A2:L51"/>
+  <dimension ref="A2:L68"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P35" sqref="P35"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6719,37 +6722,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="225" t="s">
+      <c r="A2" s="193" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="225"/>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225"/>
-      <c r="I2" s="225"/>
-      <c r="J2" s="225"/>
-      <c r="K2" s="225"/>
-      <c r="L2" s="225"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="194"/>
-      <c r="C4" s="194"/>
-      <c r="D4" s="194"/>
-      <c r="E4" s="194"/>
-      <c r="F4" s="194"/>
-      <c r="G4" s="194"/>
-      <c r="H4" s="194"/>
-      <c r="I4" s="194"/>
-      <c r="J4" s="194"/>
-      <c r="K4" s="194"/>
-      <c r="L4" s="195"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
+      <c r="H4" s="213"/>
+      <c r="I4" s="213"/>
+      <c r="J4" s="213"/>
+      <c r="K4" s="213"/>
+      <c r="L4" s="214"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="182" t="s">
@@ -6863,20 +6866,20 @@
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="194"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="195"/>
+      <c r="B9" s="213"/>
+      <c r="C9" s="213"/>
+      <c r="D9" s="213"/>
+      <c r="E9" s="213"/>
+      <c r="F9" s="213"/>
+      <c r="G9" s="213"/>
+      <c r="H9" s="213"/>
+      <c r="I9" s="213"/>
+      <c r="J9" s="213"/>
+      <c r="K9" s="213"/>
+      <c r="L9" s="214"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="182" t="s">
@@ -6990,20 +6993,20 @@
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="193" t="s">
+      <c r="A14" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="194"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="194"/>
-      <c r="E14" s="194"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="194"/>
-      <c r="H14" s="194"/>
-      <c r="I14" s="194"/>
-      <c r="J14" s="194"/>
-      <c r="K14" s="194"/>
-      <c r="L14" s="195"/>
+      <c r="B14" s="213"/>
+      <c r="C14" s="213"/>
+      <c r="D14" s="213"/>
+      <c r="E14" s="213"/>
+      <c r="F14" s="213"/>
+      <c r="G14" s="213"/>
+      <c r="H14" s="213"/>
+      <c r="I14" s="213"/>
+      <c r="J14" s="213"/>
+      <c r="K14" s="213"/>
+      <c r="L14" s="214"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="182" t="s">
@@ -7116,37 +7119,37 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A19" s="225" t="s">
+      <c r="A19" s="193" t="s">
         <v>119</v>
       </c>
-      <c r="B19" s="225"/>
-      <c r="C19" s="225"/>
-      <c r="D19" s="225"/>
-      <c r="E19" s="225"/>
-      <c r="F19" s="225"/>
-      <c r="G19" s="225"/>
-      <c r="H19" s="225"/>
-      <c r="I19" s="225"/>
-      <c r="J19" s="225"/>
-      <c r="K19" s="225"/>
-      <c r="L19" s="225"/>
+      <c r="B19" s="193"/>
+      <c r="C19" s="193"/>
+      <c r="D19" s="193"/>
+      <c r="E19" s="193"/>
+      <c r="F19" s="193"/>
+      <c r="G19" s="193"/>
+      <c r="H19" s="193"/>
+      <c r="I19" s="193"/>
+      <c r="J19" s="193"/>
+      <c r="K19" s="193"/>
+      <c r="L19" s="193"/>
     </row>
     <row r="20" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A21" s="193" t="s">
+      <c r="A21" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B21" s="194"/>
-      <c r="C21" s="194"/>
-      <c r="D21" s="194"/>
-      <c r="E21" s="194"/>
-      <c r="F21" s="194"/>
-      <c r="G21" s="194"/>
-      <c r="H21" s="194"/>
-      <c r="I21" s="194"/>
-      <c r="J21" s="194"/>
-      <c r="K21" s="194"/>
-      <c r="L21" s="195"/>
+      <c r="B21" s="213"/>
+      <c r="C21" s="213"/>
+      <c r="D21" s="213"/>
+      <c r="E21" s="213"/>
+      <c r="F21" s="213"/>
+      <c r="G21" s="213"/>
+      <c r="H21" s="213"/>
+      <c r="I21" s="213"/>
+      <c r="J21" s="213"/>
+      <c r="K21" s="213"/>
+      <c r="L21" s="214"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" s="182" t="s">
@@ -7260,20 +7263,20 @@
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="193" t="s">
+      <c r="A26" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B26" s="194"/>
-      <c r="C26" s="194"/>
-      <c r="D26" s="194"/>
-      <c r="E26" s="194"/>
-      <c r="F26" s="194"/>
-      <c r="G26" s="194"/>
-      <c r="H26" s="194"/>
-      <c r="I26" s="194"/>
-      <c r="J26" s="194"/>
-      <c r="K26" s="194"/>
-      <c r="L26" s="195"/>
+      <c r="B26" s="213"/>
+      <c r="C26" s="213"/>
+      <c r="D26" s="213"/>
+      <c r="E26" s="213"/>
+      <c r="F26" s="213"/>
+      <c r="G26" s="213"/>
+      <c r="H26" s="213"/>
+      <c r="I26" s="213"/>
+      <c r="J26" s="213"/>
+      <c r="K26" s="213"/>
+      <c r="L26" s="214"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" s="182" t="s">
@@ -7387,20 +7390,20 @@
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="31" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A31" s="193" t="s">
+      <c r="A31" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B31" s="194"/>
-      <c r="C31" s="194"/>
-      <c r="D31" s="194"/>
-      <c r="E31" s="194"/>
-      <c r="F31" s="194"/>
-      <c r="G31" s="194"/>
-      <c r="H31" s="194"/>
-      <c r="I31" s="194"/>
-      <c r="J31" s="194"/>
-      <c r="K31" s="194"/>
-      <c r="L31" s="195"/>
+      <c r="B31" s="213"/>
+      <c r="C31" s="213"/>
+      <c r="D31" s="213"/>
+      <c r="E31" s="213"/>
+      <c r="F31" s="213"/>
+      <c r="G31" s="213"/>
+      <c r="H31" s="213"/>
+      <c r="I31" s="213"/>
+      <c r="J31" s="213"/>
+      <c r="K31" s="213"/>
+      <c r="L31" s="214"/>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" s="182" t="s">
@@ -7513,37 +7516,37 @@
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A36" s="225" t="s">
+      <c r="A36" s="193" t="s">
         <v>120</v>
       </c>
-      <c r="B36" s="225"/>
-      <c r="C36" s="225"/>
-      <c r="D36" s="225"/>
-      <c r="E36" s="225"/>
-      <c r="F36" s="225"/>
-      <c r="G36" s="225"/>
-      <c r="H36" s="225"/>
-      <c r="I36" s="225"/>
-      <c r="J36" s="225"/>
-      <c r="K36" s="225"/>
-      <c r="L36" s="225"/>
+      <c r="B36" s="193"/>
+      <c r="C36" s="193"/>
+      <c r="D36" s="193"/>
+      <c r="E36" s="193"/>
+      <c r="F36" s="193"/>
+      <c r="G36" s="193"/>
+      <c r="H36" s="193"/>
+      <c r="I36" s="193"/>
+      <c r="J36" s="193"/>
+      <c r="K36" s="193"/>
+      <c r="L36" s="193"/>
     </row>
     <row r="37" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="193" t="s">
+      <c r="A38" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="194"/>
-      <c r="C38" s="194"/>
-      <c r="D38" s="194"/>
-      <c r="E38" s="194"/>
-      <c r="F38" s="194"/>
-      <c r="G38" s="194"/>
-      <c r="H38" s="194"/>
-      <c r="I38" s="194"/>
-      <c r="J38" s="194"/>
-      <c r="K38" s="194"/>
-      <c r="L38" s="195"/>
+      <c r="B38" s="213"/>
+      <c r="C38" s="213"/>
+      <c r="D38" s="213"/>
+      <c r="E38" s="213"/>
+      <c r="F38" s="213"/>
+      <c r="G38" s="213"/>
+      <c r="H38" s="213"/>
+      <c r="I38" s="213"/>
+      <c r="J38" s="213"/>
+      <c r="K38" s="213"/>
+      <c r="L38" s="214"/>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39" s="182" t="s">
@@ -7657,20 +7660,20 @@
     </row>
     <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="43" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A43" s="193" t="s">
+      <c r="A43" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B43" s="194"/>
-      <c r="C43" s="194"/>
-      <c r="D43" s="194"/>
-      <c r="E43" s="194"/>
-      <c r="F43" s="194"/>
-      <c r="G43" s="194"/>
-      <c r="H43" s="194"/>
-      <c r="I43" s="194"/>
-      <c r="J43" s="194"/>
-      <c r="K43" s="194"/>
-      <c r="L43" s="195"/>
+      <c r="B43" s="213"/>
+      <c r="C43" s="213"/>
+      <c r="D43" s="213"/>
+      <c r="E43" s="213"/>
+      <c r="F43" s="213"/>
+      <c r="G43" s="213"/>
+      <c r="H43" s="213"/>
+      <c r="I43" s="213"/>
+      <c r="J43" s="213"/>
+      <c r="K43" s="213"/>
+      <c r="L43" s="214"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="182" t="s">
@@ -7784,20 +7787,20 @@
     </row>
     <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="48" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A48" s="193" t="s">
+      <c r="A48" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="194"/>
-      <c r="C48" s="194"/>
-      <c r="D48" s="194"/>
-      <c r="E48" s="194"/>
-      <c r="F48" s="194"/>
-      <c r="G48" s="194"/>
-      <c r="H48" s="194"/>
-      <c r="I48" s="194"/>
-      <c r="J48" s="194"/>
-      <c r="K48" s="194"/>
-      <c r="L48" s="195"/>
+      <c r="B48" s="213"/>
+      <c r="C48" s="213"/>
+      <c r="D48" s="213"/>
+      <c r="E48" s="213"/>
+      <c r="F48" s="213"/>
+      <c r="G48" s="213"/>
+      <c r="H48" s="213"/>
+      <c r="I48" s="213"/>
+      <c r="J48" s="213"/>
+      <c r="K48" s="213"/>
+      <c r="L48" s="214"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" s="182" t="s">
@@ -7909,8 +7912,408 @@
         <v>5.357279084551811</v>
       </c>
     </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="193" t="s">
+        <v>121</v>
+      </c>
+      <c r="B53" s="193"/>
+      <c r="C53" s="193"/>
+      <c r="D53" s="193"/>
+      <c r="E53" s="193"/>
+      <c r="F53" s="193"/>
+      <c r="G53" s="193"/>
+      <c r="H53" s="193"/>
+      <c r="I53" s="193"/>
+      <c r="J53" s="193"/>
+      <c r="K53" s="193"/>
+      <c r="L53" s="193"/>
+    </row>
+    <row r="54" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A55" s="212" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="213"/>
+      <c r="C55" s="213"/>
+      <c r="D55" s="213"/>
+      <c r="E55" s="213"/>
+      <c r="F55" s="213"/>
+      <c r="G55" s="213"/>
+      <c r="H55" s="213"/>
+      <c r="I55" s="213"/>
+      <c r="J55" s="213"/>
+      <c r="K55" s="213"/>
+      <c r="L55" s="214"/>
+    </row>
+    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A56" s="182" t="s">
+        <v>89</v>
+      </c>
+      <c r="B56" s="186"/>
+      <c r="C56" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D56" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F56" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G56" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H56" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I56" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J56" s="178"/>
+      <c r="K56" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L56" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="183">
+        <v>72400000</v>
+      </c>
+      <c r="B57" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C57" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D57" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E57" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F57" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G57" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H57" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I57" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J57" s="180"/>
+      <c r="K57" s="184">
+        <f>(H57/(A57*C57*D57*E57*F57))-1</f>
+        <v>2.7531149124227055</v>
+      </c>
+      <c r="L57" s="185">
+        <f>(I57/(A57*C57*D57*E57*G57))-1</f>
+        <v>2.8811013195744484</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="183">
+        <v>40800000</v>
+      </c>
+      <c r="B58" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C58" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D58" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E58" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F58" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G58" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H58" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I58" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J58" s="180"/>
+      <c r="K58" s="184">
+        <f>(H58/(A58*C58*D58*E58*F58))-1</f>
+        <v>5.659939207338331</v>
+      </c>
+      <c r="L58" s="185">
+        <f>(I58/(A58*C58*D58*E58*G58))-1</f>
+        <v>5.8870523415977951</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A60" s="212" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" s="213"/>
+      <c r="C60" s="213"/>
+      <c r="D60" s="213"/>
+      <c r="E60" s="213"/>
+      <c r="F60" s="213"/>
+      <c r="G60" s="213"/>
+      <c r="H60" s="213"/>
+      <c r="I60" s="213"/>
+      <c r="J60" s="213"/>
+      <c r="K60" s="213"/>
+      <c r="L60" s="214"/>
+    </row>
+    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A61" s="182" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="186"/>
+      <c r="C61" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D61" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E61" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F61" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G61" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H61" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I61" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J61" s="178"/>
+      <c r="K61" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L61" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="183">
+        <v>84400000</v>
+      </c>
+      <c r="B62" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D62" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E62" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F62" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G62" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H62" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I62" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J62" s="180"/>
+      <c r="K62" s="184">
+        <f>(H62/(A62*C62*D62*E62*F62))-1</f>
+        <v>2.219496678428956</v>
+      </c>
+      <c r="L62" s="184">
+        <f>(I62/(A62*C62*D62*E62*G62))-1</f>
+        <v>2.3292859660804504</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="183">
+        <v>65600000</v>
+      </c>
+      <c r="B63" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D63" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E63" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F63" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G63" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H63" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I63" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J63" s="180"/>
+      <c r="K63" s="184">
+        <f>(H63/(A63*C63*D63*E63*F63))-1</f>
+        <v>3.1421573118811565</v>
+      </c>
+      <c r="L63" s="184">
+        <f>(I63/(A63*C63*D63*E63*G63))-1</f>
+        <v>3.2834106027010677</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A65" s="212" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="213"/>
+      <c r="C65" s="213"/>
+      <c r="D65" s="213"/>
+      <c r="E65" s="213"/>
+      <c r="F65" s="213"/>
+      <c r="G65" s="213"/>
+      <c r="H65" s="213"/>
+      <c r="I65" s="213"/>
+      <c r="J65" s="213"/>
+      <c r="K65" s="213"/>
+      <c r="L65" s="214"/>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A66" s="182" t="s">
+        <v>99</v>
+      </c>
+      <c r="B66" s="186"/>
+      <c r="C66" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D66" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E66" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F66" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G66" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H66" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I66" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J66" s="178"/>
+      <c r="K66" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L66" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A67" s="183">
+        <v>84400000</v>
+      </c>
+      <c r="B67" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C67" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D67" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E67" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F67" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G67" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H67" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I67" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J67" s="180"/>
+      <c r="K67" s="184">
+        <f>(H67/(A67*C67*D67*E67*F67))-1</f>
+        <v>2.219496678428956</v>
+      </c>
+      <c r="L67" s="185">
+        <f>(I67/(A67*C67*D67*E67*G67))-1</f>
+        <v>2.3292859660804504</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="183">
+        <v>46200000</v>
+      </c>
+      <c r="B68" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C68" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D68" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E68" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F68" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G68" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H68" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I68" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J68" s="180"/>
+      <c r="K68" s="184">
+        <f>(H68/(A68*C68*D68*E68*F68))-1</f>
+        <v>4.8815047545325507</v>
+      </c>
+      <c r="L68" s="185">
+        <f>(I68/(A68*C68*D68*E68*G68))-1</f>
+        <v>5.0820721977746759</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="12">
+    <mergeCell ref="A55:L55"/>
+    <mergeCell ref="A60:L60"/>
+    <mergeCell ref="A65:L65"/>
     <mergeCell ref="A38:L38"/>
     <mergeCell ref="A43:L43"/>
     <mergeCell ref="A48:L48"/>
@@ -7940,37 +8343,37 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" s="225" t="s">
+      <c r="A2" s="193" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="225"/>
-      <c r="C2" s="225"/>
-      <c r="D2" s="225"/>
-      <c r="E2" s="225"/>
-      <c r="F2" s="225"/>
-      <c r="G2" s="225"/>
-      <c r="H2" s="225"/>
-      <c r="I2" s="225"/>
-      <c r="J2" s="225"/>
-      <c r="K2" s="225"/>
-      <c r="L2" s="225"/>
+      <c r="B2" s="193"/>
+      <c r="C2" s="193"/>
+      <c r="D2" s="193"/>
+      <c r="E2" s="193"/>
+      <c r="F2" s="193"/>
+      <c r="G2" s="193"/>
+      <c r="H2" s="193"/>
+      <c r="I2" s="193"/>
+      <c r="J2" s="193"/>
+      <c r="K2" s="193"/>
+      <c r="L2" s="193"/>
     </row>
     <row r="3" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="193" t="s">
+      <c r="A4" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="194"/>
-      <c r="C4" s="194"/>
-      <c r="D4" s="194"/>
-      <c r="E4" s="194"/>
-      <c r="F4" s="194"/>
-      <c r="G4" s="194"/>
-      <c r="H4" s="194"/>
-      <c r="I4" s="194"/>
-      <c r="J4" s="194"/>
-      <c r="K4" s="194"/>
-      <c r="L4" s="195"/>
+      <c r="B4" s="213"/>
+      <c r="C4" s="213"/>
+      <c r="D4" s="213"/>
+      <c r="E4" s="213"/>
+      <c r="F4" s="213"/>
+      <c r="G4" s="213"/>
+      <c r="H4" s="213"/>
+      <c r="I4" s="213"/>
+      <c r="J4" s="213"/>
+      <c r="K4" s="213"/>
+      <c r="L4" s="214"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="182" t="s">
@@ -8084,20 +8487,20 @@
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="9" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A9" s="193" t="s">
+      <c r="A9" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B9" s="194"/>
-      <c r="C9" s="194"/>
-      <c r="D9" s="194"/>
-      <c r="E9" s="194"/>
-      <c r="F9" s="194"/>
-      <c r="G9" s="194"/>
-      <c r="H9" s="194"/>
-      <c r="I9" s="194"/>
-      <c r="J9" s="194"/>
-      <c r="K9" s="194"/>
-      <c r="L9" s="195"/>
+      <c r="B9" s="213"/>
+      <c r="C9" s="213"/>
+      <c r="D9" s="213"/>
+      <c r="E9" s="213"/>
+      <c r="F9" s="213"/>
+      <c r="G9" s="213"/>
+      <c r="H9" s="213"/>
+      <c r="I9" s="213"/>
+      <c r="J9" s="213"/>
+      <c r="K9" s="213"/>
+      <c r="L9" s="214"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="182" t="s">
@@ -8211,20 +8614,20 @@
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="14" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A14" s="193" t="s">
+      <c r="A14" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="194"/>
-      <c r="C14" s="194"/>
-      <c r="D14" s="194"/>
-      <c r="E14" s="194"/>
-      <c r="F14" s="194"/>
-      <c r="G14" s="194"/>
-      <c r="H14" s="194"/>
-      <c r="I14" s="194"/>
-      <c r="J14" s="194"/>
-      <c r="K14" s="194"/>
-      <c r="L14" s="195"/>
+      <c r="B14" s="213"/>
+      <c r="C14" s="213"/>
+      <c r="D14" s="213"/>
+      <c r="E14" s="213"/>
+      <c r="F14" s="213"/>
+      <c r="G14" s="213"/>
+      <c r="H14" s="213"/>
+      <c r="I14" s="213"/>
+      <c r="J14" s="213"/>
+      <c r="K14" s="213"/>
+      <c r="L14" s="214"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="182" t="s">
@@ -8337,37 +8740,37 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="225" t="s">
+      <c r="A20" s="193" t="s">
         <v>117</v>
       </c>
-      <c r="B20" s="225"/>
-      <c r="C20" s="225"/>
-      <c r="D20" s="225"/>
-      <c r="E20" s="225"/>
-      <c r="F20" s="225"/>
-      <c r="G20" s="225"/>
-      <c r="H20" s="225"/>
-      <c r="I20" s="225"/>
-      <c r="J20" s="225"/>
-      <c r="K20" s="225"/>
-      <c r="L20" s="225"/>
+      <c r="B20" s="193"/>
+      <c r="C20" s="193"/>
+      <c r="D20" s="193"/>
+      <c r="E20" s="193"/>
+      <c r="F20" s="193"/>
+      <c r="G20" s="193"/>
+      <c r="H20" s="193"/>
+      <c r="I20" s="193"/>
+      <c r="J20" s="193"/>
+      <c r="K20" s="193"/>
+      <c r="L20" s="193"/>
     </row>
     <row r="21" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A22" s="193" t="s">
+      <c r="A22" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B22" s="194"/>
-      <c r="C22" s="194"/>
-      <c r="D22" s="194"/>
-      <c r="E22" s="194"/>
-      <c r="F22" s="194"/>
-      <c r="G22" s="194"/>
-      <c r="H22" s="194"/>
-      <c r="I22" s="194"/>
-      <c r="J22" s="194"/>
-      <c r="K22" s="194"/>
-      <c r="L22" s="195"/>
+      <c r="B22" s="213"/>
+      <c r="C22" s="213"/>
+      <c r="D22" s="213"/>
+      <c r="E22" s="213"/>
+      <c r="F22" s="213"/>
+      <c r="G22" s="213"/>
+      <c r="H22" s="213"/>
+      <c r="I22" s="213"/>
+      <c r="J22" s="213"/>
+      <c r="K22" s="213"/>
+      <c r="L22" s="214"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" s="182" t="s">
@@ -8481,20 +8884,20 @@
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A27" s="193" t="s">
+      <c r="A27" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="194"/>
-      <c r="C27" s="194"/>
-      <c r="D27" s="194"/>
-      <c r="E27" s="194"/>
-      <c r="F27" s="194"/>
-      <c r="G27" s="194"/>
-      <c r="H27" s="194"/>
-      <c r="I27" s="194"/>
-      <c r="J27" s="194"/>
-      <c r="K27" s="194"/>
-      <c r="L27" s="195"/>
+      <c r="B27" s="213"/>
+      <c r="C27" s="213"/>
+      <c r="D27" s="213"/>
+      <c r="E27" s="213"/>
+      <c r="F27" s="213"/>
+      <c r="G27" s="213"/>
+      <c r="H27" s="213"/>
+      <c r="I27" s="213"/>
+      <c r="J27" s="213"/>
+      <c r="K27" s="213"/>
+      <c r="L27" s="214"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" s="182" t="s">
@@ -8608,20 +9011,20 @@
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A32" s="193" t="s">
+      <c r="A32" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B32" s="194"/>
-      <c r="C32" s="194"/>
-      <c r="D32" s="194"/>
-      <c r="E32" s="194"/>
-      <c r="F32" s="194"/>
-      <c r="G32" s="194"/>
-      <c r="H32" s="194"/>
-      <c r="I32" s="194"/>
-      <c r="J32" s="194"/>
-      <c r="K32" s="194"/>
-      <c r="L32" s="195"/>
+      <c r="B32" s="213"/>
+      <c r="C32" s="213"/>
+      <c r="D32" s="213"/>
+      <c r="E32" s="213"/>
+      <c r="F32" s="213"/>
+      <c r="G32" s="213"/>
+      <c r="H32" s="213"/>
+      <c r="I32" s="213"/>
+      <c r="J32" s="213"/>
+      <c r="K32" s="213"/>
+      <c r="L32" s="214"/>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" s="182" t="s">
@@ -8734,37 +9137,37 @@
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A38" s="225" t="s">
+      <c r="A38" s="193" t="s">
         <v>117</v>
       </c>
-      <c r="B38" s="225"/>
-      <c r="C38" s="225"/>
-      <c r="D38" s="225"/>
-      <c r="E38" s="225"/>
-      <c r="F38" s="225"/>
-      <c r="G38" s="225"/>
-      <c r="H38" s="225"/>
-      <c r="I38" s="225"/>
-      <c r="J38" s="225"/>
-      <c r="K38" s="225"/>
-      <c r="L38" s="225"/>
+      <c r="B38" s="193"/>
+      <c r="C38" s="193"/>
+      <c r="D38" s="193"/>
+      <c r="E38" s="193"/>
+      <c r="F38" s="193"/>
+      <c r="G38" s="193"/>
+      <c r="H38" s="193"/>
+      <c r="I38" s="193"/>
+      <c r="J38" s="193"/>
+      <c r="K38" s="193"/>
+      <c r="L38" s="193"/>
     </row>
     <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="40" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A40" s="193" t="s">
+      <c r="A40" s="212" t="s">
         <v>88</v>
       </c>
-      <c r="B40" s="194"/>
-      <c r="C40" s="194"/>
-      <c r="D40" s="194"/>
-      <c r="E40" s="194"/>
-      <c r="F40" s="194"/>
-      <c r="G40" s="194"/>
-      <c r="H40" s="194"/>
-      <c r="I40" s="194"/>
-      <c r="J40" s="194"/>
-      <c r="K40" s="194"/>
-      <c r="L40" s="195"/>
+      <c r="B40" s="213"/>
+      <c r="C40" s="213"/>
+      <c r="D40" s="213"/>
+      <c r="E40" s="213"/>
+      <c r="F40" s="213"/>
+      <c r="G40" s="213"/>
+      <c r="H40" s="213"/>
+      <c r="I40" s="213"/>
+      <c r="J40" s="213"/>
+      <c r="K40" s="213"/>
+      <c r="L40" s="214"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41" s="182" t="s">
@@ -8878,20 +9281,20 @@
     </row>
     <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="45" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A45" s="193" t="s">
+      <c r="A45" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B45" s="194"/>
-      <c r="C45" s="194"/>
-      <c r="D45" s="194"/>
-      <c r="E45" s="194"/>
-      <c r="F45" s="194"/>
-      <c r="G45" s="194"/>
-      <c r="H45" s="194"/>
-      <c r="I45" s="194"/>
-      <c r="J45" s="194"/>
-      <c r="K45" s="194"/>
-      <c r="L45" s="195"/>
+      <c r="B45" s="213"/>
+      <c r="C45" s="213"/>
+      <c r="D45" s="213"/>
+      <c r="E45" s="213"/>
+      <c r="F45" s="213"/>
+      <c r="G45" s="213"/>
+      <c r="H45" s="213"/>
+      <c r="I45" s="213"/>
+      <c r="J45" s="213"/>
+      <c r="K45" s="213"/>
+      <c r="L45" s="214"/>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46" s="182" t="s">
@@ -9005,20 +9408,20 @@
     </row>
     <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="50" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A50" s="193" t="s">
+      <c r="A50" s="212" t="s">
         <v>101</v>
       </c>
-      <c r="B50" s="194"/>
-      <c r="C50" s="194"/>
-      <c r="D50" s="194"/>
-      <c r="E50" s="194"/>
-      <c r="F50" s="194"/>
-      <c r="G50" s="194"/>
-      <c r="H50" s="194"/>
-      <c r="I50" s="194"/>
-      <c r="J50" s="194"/>
-      <c r="K50" s="194"/>
-      <c r="L50" s="195"/>
+      <c r="B50" s="213"/>
+      <c r="C50" s="213"/>
+      <c r="D50" s="213"/>
+      <c r="E50" s="213"/>
+      <c r="F50" s="213"/>
+      <c r="G50" s="213"/>
+      <c r="H50" s="213"/>
+      <c r="I50" s="213"/>
+      <c r="J50" s="213"/>
+      <c r="K50" s="213"/>
+      <c r="L50" s="214"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" s="182" t="s">
@@ -9150,7 +9553,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{519799BC-EE76-4C42-A73D-AC4D7E6854EE}">
   <dimension ref="A1:AF28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
@@ -9179,54 +9582,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="25.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="222" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="207" t="s">
+      <c r="C1" s="238" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="208"/>
-      <c r="E1" s="208"/>
-      <c r="F1" s="209"/>
-      <c r="H1" s="210" t="s">
+      <c r="D1" s="239"/>
+      <c r="E1" s="239"/>
+      <c r="F1" s="240"/>
+      <c r="H1" s="241" t="s">
         <v>46</v>
       </c>
-      <c r="I1" s="211"/>
-      <c r="J1" s="211"/>
-      <c r="K1" s="212"/>
-      <c r="L1" s="213" t="s">
+      <c r="I1" s="242"/>
+      <c r="J1" s="242"/>
+      <c r="K1" s="243"/>
+      <c r="L1" s="244" t="s">
         <v>48</v>
       </c>
-      <c r="M1" s="214"/>
-      <c r="N1" s="214"/>
-      <c r="O1" s="240"/>
-      <c r="Q1" s="215" t="s">
+      <c r="M1" s="245"/>
+      <c r="N1" s="245"/>
+      <c r="O1" s="246"/>
+      <c r="Q1" s="247" t="s">
         <v>47</v>
       </c>
-      <c r="R1" s="216"/>
-      <c r="S1" s="216"/>
-      <c r="T1" s="217"/>
-      <c r="U1" s="218" t="s">
+      <c r="R1" s="248"/>
+      <c r="S1" s="248"/>
+      <c r="T1" s="249"/>
+      <c r="U1" s="250" t="s">
         <v>49</v>
       </c>
-      <c r="V1" s="219"/>
-      <c r="W1" s="219"/>
-      <c r="X1" s="220"/>
-      <c r="Y1" s="198" t="s">
+      <c r="V1" s="251"/>
+      <c r="W1" s="251"/>
+      <c r="X1" s="252"/>
+      <c r="Y1" s="236" t="s">
         <v>70</v>
       </c>
-      <c r="Z1" s="199"/>
-      <c r="AA1" s="199"/>
-      <c r="AB1" s="200"/>
-      <c r="AC1" s="221" t="s">
+      <c r="Z1" s="225"/>
+      <c r="AA1" s="225"/>
+      <c r="AB1" s="226"/>
+      <c r="AC1" s="224" t="s">
         <v>71</v>
       </c>
-      <c r="AD1" s="199"/>
-      <c r="AE1" s="199"/>
-      <c r="AF1" s="200"/>
+      <c r="AD1" s="225"/>
+      <c r="AE1" s="225"/>
+      <c r="AF1" s="226"/>
     </row>
     <row r="2" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="233"/>
+      <c r="A2" s="223"/>
       <c r="C2" s="52" t="s">
         <v>60</v>
       </c>
@@ -9260,7 +9663,7 @@
       <c r="N2" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="O2" s="241" t="s">
+      <c r="O2" s="202" t="s">
         <v>65</v>
       </c>
       <c r="Q2" s="60" t="s">
@@ -9287,17 +9690,17 @@
       <c r="X2" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="Y2" s="201"/>
-      <c r="Z2" s="202"/>
-      <c r="AA2" s="202"/>
-      <c r="AB2" s="203"/>
-      <c r="AC2" s="222"/>
-      <c r="AD2" s="202"/>
-      <c r="AE2" s="202"/>
-      <c r="AF2" s="203"/>
+      <c r="Y2" s="237"/>
+      <c r="Z2" s="228"/>
+      <c r="AA2" s="228"/>
+      <c r="AB2" s="229"/>
+      <c r="AC2" s="227"/>
+      <c r="AD2" s="228"/>
+      <c r="AE2" s="228"/>
+      <c r="AF2" s="229"/>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A3" s="234" t="s">
+      <c r="A3" s="196" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="152">
@@ -9324,12 +9727,12 @@
         <v>59</v>
       </c>
       <c r="M3" s="91">
-        <f>(I3-D3)/D3*100</f>
+        <f t="shared" ref="M3:M11" si="0">(I3-D3)/D3*100</f>
         <v>-10.472047244094499</v>
       </c>
       <c r="N3" s="91"/>
-      <c r="O3" s="242">
-        <f>(K3-F3)/F3*100</f>
+      <c r="O3" s="203">
+        <f t="shared" ref="O3:O11" si="1">(K3-F3)/F3*100</f>
         <v>-11.633045786330527</v>
       </c>
       <c r="Q3" s="154">
@@ -9347,25 +9750,25 @@
         <v>59</v>
       </c>
       <c r="V3" s="92">
-        <f>(R3-D3)/D3*100</f>
+        <f t="shared" ref="V3:V9" si="2">(R3-D3)/D3*100</f>
         <v>-32.332480314960641</v>
       </c>
       <c r="W3" s="92"/>
       <c r="X3" s="93">
-        <f>(T3-F3)/F3*100</f>
+        <f t="shared" ref="X3:X9" si="3">(T3-F3)/F3*100</f>
         <v>11.731652289316489</v>
       </c>
-      <c r="Y3" s="204"/>
-      <c r="Z3" s="205"/>
-      <c r="AA3" s="205"/>
-      <c r="AB3" s="206"/>
-      <c r="AC3" s="223"/>
-      <c r="AD3" s="205"/>
-      <c r="AE3" s="205"/>
-      <c r="AF3" s="206"/>
+      <c r="Y3" s="221"/>
+      <c r="Z3" s="219"/>
+      <c r="AA3" s="219"/>
+      <c r="AB3" s="220"/>
+      <c r="AC3" s="218"/>
+      <c r="AD3" s="219"/>
+      <c r="AE3" s="219"/>
+      <c r="AF3" s="220"/>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A4" s="235" t="s">
+      <c r="A4" s="197" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="116" t="s">
@@ -9388,12 +9791,12 @@
         <v>59</v>
       </c>
       <c r="M4" s="123">
-        <f>(I4-D4)/D4*100</f>
+        <f t="shared" si="0"/>
         <v>-100</v>
       </c>
       <c r="N4" s="123"/>
-      <c r="O4" s="243">
-        <f>(K4-F4)/F4*100</f>
+      <c r="O4" s="204">
+        <f t="shared" si="1"/>
         <v>-100</v>
       </c>
       <c r="Q4" s="124" t="s">
@@ -9406,25 +9809,25 @@
         <v>59</v>
       </c>
       <c r="V4" s="95">
-        <f>(R4-D4)/D4*100</f>
+        <f t="shared" si="2"/>
         <v>-100</v>
       </c>
       <c r="W4" s="95"/>
       <c r="X4" s="96">
-        <f>(T4-F4)/F4*100</f>
+        <f t="shared" si="3"/>
         <v>-100</v>
       </c>
-      <c r="Y4" s="204"/>
-      <c r="Z4" s="205"/>
-      <c r="AA4" s="205"/>
-      <c r="AB4" s="206"/>
-      <c r="AC4" s="223"/>
-      <c r="AD4" s="205"/>
-      <c r="AE4" s="205"/>
-      <c r="AF4" s="206"/>
+      <c r="Y4" s="221"/>
+      <c r="Z4" s="219"/>
+      <c r="AA4" s="219"/>
+      <c r="AB4" s="220"/>
+      <c r="AC4" s="218"/>
+      <c r="AD4" s="219"/>
+      <c r="AE4" s="219"/>
+      <c r="AF4" s="220"/>
     </row>
     <row r="5" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="236" t="s">
+      <c r="A5" s="198" t="s">
         <v>36</v>
       </c>
       <c r="C5" s="127" t="s">
@@ -9452,12 +9855,12 @@
         <v>59</v>
       </c>
       <c r="M5" s="88">
-        <f>(I5-D5)/D5*100</f>
+        <f t="shared" si="0"/>
         <v>-22.472309711286094</v>
       </c>
       <c r="N5" s="88"/>
       <c r="O5" s="87">
-        <f>(K5-F5)/F5*100</f>
+        <f t="shared" si="1"/>
         <v>-29.747710683477141</v>
       </c>
       <c r="Q5" s="131" t="s">
@@ -9475,25 +9878,25 @@
         <v>59</v>
       </c>
       <c r="V5" s="97">
-        <f>(R5-D5)/D5*100</f>
+        <f t="shared" si="2"/>
         <v>-26.861220472440948</v>
       </c>
       <c r="W5" s="97"/>
       <c r="X5" s="98">
-        <f>(T5-F5)/F5*100</f>
+        <f t="shared" si="3"/>
         <v>-31.876045122760488</v>
       </c>
-      <c r="Y5" s="204"/>
-      <c r="Z5" s="205"/>
-      <c r="AA5" s="205"/>
-      <c r="AB5" s="206"/>
-      <c r="AC5" s="223"/>
-      <c r="AD5" s="205"/>
-      <c r="AE5" s="205"/>
-      <c r="AF5" s="206"/>
+      <c r="Y5" s="221"/>
+      <c r="Z5" s="219"/>
+      <c r="AA5" s="219"/>
+      <c r="AB5" s="220"/>
+      <c r="AC5" s="218"/>
+      <c r="AD5" s="219"/>
+      <c r="AE5" s="219"/>
+      <c r="AF5" s="220"/>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="236" t="s">
+      <c r="A6" s="198" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="132">
@@ -9522,12 +9925,12 @@
         <v>-33.333333333333329</v>
       </c>
       <c r="M6" s="72">
-        <f>(I6-D6)/D6*100</f>
+        <f t="shared" si="0"/>
         <v>-6.5654855643044572</v>
       </c>
       <c r="N6" s="72"/>
-      <c r="O6" s="244">
-        <f>(K6-F6)/F6*100</f>
+      <c r="O6" s="205">
+        <f t="shared" si="1"/>
         <v>-7.4755142667551748</v>
       </c>
       <c r="Q6" s="80">
@@ -9546,25 +9949,25 @@
         <v>33.333333333333329</v>
       </c>
       <c r="V6" s="77">
-        <f>(R6-D6)/D6*100</f>
+        <f t="shared" si="2"/>
         <v>6.3526246719160078</v>
       </c>
       <c r="W6" s="77"/>
       <c r="X6" s="99">
-        <f>(T6-F6)/F6*100</f>
+        <f t="shared" si="3"/>
         <v>7.5742534837425071</v>
       </c>
-      <c r="Y6" s="204"/>
-      <c r="Z6" s="205"/>
-      <c r="AA6" s="205"/>
-      <c r="AB6" s="206"/>
-      <c r="AC6" s="223"/>
-      <c r="AD6" s="205"/>
-      <c r="AE6" s="205"/>
-      <c r="AF6" s="206"/>
+      <c r="Y6" s="221"/>
+      <c r="Z6" s="219"/>
+      <c r="AA6" s="219"/>
+      <c r="AB6" s="220"/>
+      <c r="AC6" s="218"/>
+      <c r="AD6" s="219"/>
+      <c r="AE6" s="219"/>
+      <c r="AF6" s="220"/>
     </row>
     <row r="7" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="236" t="s">
+      <c r="A7" s="198" t="s">
         <v>67</v>
       </c>
       <c r="C7" s="127">
@@ -9592,12 +9995,12 @@
         <v>-46.153846153846153</v>
       </c>
       <c r="M7" s="91">
-        <f>(I7-D7)/D7*100</f>
+        <f t="shared" si="0"/>
         <v>-20.347769028871394</v>
       </c>
       <c r="N7" s="91"/>
-      <c r="O7" s="242">
-        <f>(K7-F7)/F7*100</f>
+      <c r="O7" s="203">
+        <f t="shared" si="1"/>
         <v>-26.914399469144001</v>
       </c>
       <c r="Q7" s="115">
@@ -9616,25 +10019,25 @@
         <v>15.384615384615385</v>
       </c>
       <c r="V7" s="92">
-        <f>(R7-D7)/D7*100</f>
+        <f t="shared" si="2"/>
         <v>5.5280183727034133</v>
       </c>
       <c r="W7" s="92"/>
       <c r="X7" s="98">
-        <f>(T7-F7)/F7*100</f>
+        <f t="shared" si="3"/>
         <v>9.0357000663569984</v>
       </c>
-      <c r="Y7" s="204"/>
-      <c r="Z7" s="205"/>
-      <c r="AA7" s="205"/>
-      <c r="AB7" s="206"/>
-      <c r="AC7" s="223"/>
-      <c r="AD7" s="205"/>
-      <c r="AE7" s="205"/>
-      <c r="AF7" s="206"/>
+      <c r="Y7" s="221"/>
+      <c r="Z7" s="219"/>
+      <c r="AA7" s="219"/>
+      <c r="AB7" s="220"/>
+      <c r="AC7" s="218"/>
+      <c r="AD7" s="219"/>
+      <c r="AE7" s="219"/>
+      <c r="AF7" s="220"/>
     </row>
     <row r="8" spans="1:32" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="236" t="s">
+      <c r="A8" s="198" t="s">
         <v>68</v>
       </c>
       <c r="C8" s="127">
@@ -9663,12 +10066,12 @@
         <v>-36.666666666666664</v>
       </c>
       <c r="M8" s="88">
-        <f>(I8-D8)/D8*100</f>
+        <f t="shared" si="0"/>
         <v>-0.80065616797900618</v>
       </c>
       <c r="N8" s="88"/>
       <c r="O8" s="87">
-        <f>(K8-F8)/F8*100</f>
+        <f t="shared" si="1"/>
         <v>-6.9404114134041297</v>
       </c>
       <c r="Q8" s="131">
@@ -9687,25 +10090,25 @@
         <v>13.333333333333334</v>
       </c>
       <c r="V8" s="97">
-        <f>(R8-D8)/D8*100</f>
+        <f t="shared" si="2"/>
         <v>0.26745406824147122</v>
       </c>
       <c r="W8" s="97"/>
       <c r="X8" s="98">
-        <f>(T8-F8)/F8*100</f>
+        <f t="shared" si="3"/>
         <v>2.5911081619110119</v>
       </c>
-      <c r="Y8" s="204"/>
-      <c r="Z8" s="205"/>
-      <c r="AA8" s="205"/>
-      <c r="AB8" s="206"/>
-      <c r="AC8" s="223"/>
-      <c r="AD8" s="205"/>
-      <c r="AE8" s="205"/>
-      <c r="AF8" s="206"/>
+      <c r="Y8" s="221"/>
+      <c r="Z8" s="219"/>
+      <c r="AA8" s="219"/>
+      <c r="AB8" s="220"/>
+      <c r="AC8" s="218"/>
+      <c r="AD8" s="219"/>
+      <c r="AE8" s="219"/>
+      <c r="AF8" s="220"/>
     </row>
     <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="237" t="s">
+      <c r="A9" s="199" t="s">
         <v>75</v>
       </c>
       <c r="C9" s="132">
@@ -9734,12 +10137,12 @@
         <v>-31.578947368421051</v>
       </c>
       <c r="M9" s="72">
-        <f>(I9-D9)/D9*100</f>
+        <f t="shared" si="0"/>
         <v>-32.359973753280848</v>
       </c>
       <c r="N9" s="72"/>
-      <c r="O9" s="244">
-        <f>(K9-F9)/F9*100</f>
+      <c r="O9" s="205">
+        <f t="shared" si="1"/>
         <v>-24.416323822163307</v>
       </c>
       <c r="Q9" s="137">
@@ -9758,25 +10161,25 @@
         <v>-10.526315789473683</v>
       </c>
       <c r="V9" s="100">
-        <f>(R9-D9)/D9*100</f>
+        <f t="shared" si="2"/>
         <v>-10.671981627296596</v>
       </c>
       <c r="W9" s="100"/>
       <c r="X9" s="101">
-        <f>(T9-F9)/F9*100</f>
+        <f t="shared" si="3"/>
         <v>-8.1059057730590833</v>
       </c>
-      <c r="Y9" s="204"/>
-      <c r="Z9" s="205"/>
-      <c r="AA9" s="205"/>
-      <c r="AB9" s="206"/>
-      <c r="AC9" s="223"/>
-      <c r="AD9" s="205"/>
-      <c r="AE9" s="205"/>
-      <c r="AF9" s="206"/>
+      <c r="Y9" s="221"/>
+      <c r="Z9" s="219"/>
+      <c r="AA9" s="219"/>
+      <c r="AB9" s="220"/>
+      <c r="AC9" s="218"/>
+      <c r="AD9" s="219"/>
+      <c r="AE9" s="219"/>
+      <c r="AF9" s="220"/>
     </row>
     <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="238" t="s">
+      <c r="A10" s="200" t="s">
         <v>63</v>
       </c>
       <c r="C10" s="151">
@@ -9804,12 +10207,12 @@
         <v>59</v>
       </c>
       <c r="M10" s="140">
-        <f>(I10-D10)/D10*100</f>
+        <f t="shared" si="0"/>
         <v>24.110564304461935</v>
       </c>
       <c r="N10" s="140"/>
-      <c r="O10" s="245">
-        <f>(K10-F10)/F10*100</f>
+      <c r="O10" s="206">
+        <f t="shared" si="1"/>
         <v>4.9369608493665888E-2</v>
       </c>
       <c r="Q10" s="131" t="s">
@@ -9844,7 +10247,7 @@
       <c r="AF10" s="69"/>
     </row>
     <row r="11" spans="1:32" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="239" t="s">
+      <c r="A11" s="201" t="s">
         <v>53</v>
       </c>
       <c r="C11" s="141">
@@ -9871,12 +10274,12 @@
         <v>0.5</v>
       </c>
       <c r="M11" s="70">
-        <f>(I11-D11)/D11*100</f>
+        <f t="shared" si="0"/>
         <v>9.6456692913385744</v>
       </c>
       <c r="N11" s="70"/>
-      <c r="O11" s="246">
-        <f>(K11-F11)/F11*100</f>
+      <c r="O11" s="207">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q11" s="148" t="s">
@@ -9899,16 +10302,16 @@
       <c r="X11" s="104" t="s">
         <v>59</v>
       </c>
-      <c r="Y11" s="196" t="s">
+      <c r="Y11" s="216" t="s">
         <v>69</v>
       </c>
-      <c r="Z11" s="196"/>
-      <c r="AA11" s="196"/>
-      <c r="AB11" s="197"/>
-      <c r="AC11" s="224"/>
-      <c r="AD11" s="196"/>
-      <c r="AE11" s="196"/>
-      <c r="AF11" s="197"/>
+      <c r="Z11" s="216"/>
+      <c r="AA11" s="216"/>
+      <c r="AB11" s="217"/>
+      <c r="AC11" s="215"/>
+      <c r="AD11" s="216"/>
+      <c r="AE11" s="216"/>
+      <c r="AF11" s="217"/>
     </row>
     <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12" s="82" t="s">
@@ -9935,40 +10338,40 @@
       </c>
     </row>
     <row r="15" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A15" s="226" t="s">
+      <c r="A15" s="194" t="s">
         <v>34</v>
       </c>
-      <c r="B15" s="247"/>
-      <c r="C15" s="227" t="s">
+      <c r="B15" s="208"/>
+      <c r="C15" s="234" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="227"/>
-      <c r="E15" s="228"/>
+      <c r="D15" s="234"/>
+      <c r="E15" s="235"/>
       <c r="J15" s="49"/>
     </row>
     <row r="16" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A16" s="248" t="s">
+      <c r="A16" s="209" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="251"/>
-      <c r="C16" s="249" t="s">
+      <c r="B16" s="210"/>
+      <c r="C16" s="230" t="s">
         <v>57</v>
       </c>
-      <c r="D16" s="249"/>
-      <c r="E16" s="250"/>
+      <c r="D16" s="230"/>
+      <c r="E16" s="231"/>
       <c r="I16" s="50"/>
       <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.3">
-      <c r="A17" s="229" t="s">
+      <c r="A17" s="195" t="s">
         <v>55</v>
       </c>
-      <c r="B17" s="252"/>
-      <c r="C17" s="230" t="s">
+      <c r="B17" s="211"/>
+      <c r="C17" s="232" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="230"/>
-      <c r="E17" s="231"/>
+      <c r="D17" s="232"/>
+      <c r="E17" s="233"/>
       <c r="H17" t="s">
         <v>58</v>
       </c>
@@ -10020,17 +10423,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="AC11:AF11"/>
-    <mergeCell ref="AC6:AF6"/>
-    <mergeCell ref="AC7:AF7"/>
-    <mergeCell ref="AC8:AF8"/>
-    <mergeCell ref="AC9:AF9"/>
-    <mergeCell ref="Y9:AB9"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="AC1:AF2"/>
-    <mergeCell ref="AC3:AF3"/>
-    <mergeCell ref="AC4:AF4"/>
-    <mergeCell ref="AC5:AF5"/>
     <mergeCell ref="Y11:AB11"/>
     <mergeCell ref="C16:E16"/>
     <mergeCell ref="C17:E17"/>
@@ -10047,6 +10439,17 @@
     <mergeCell ref="Q1:T1"/>
     <mergeCell ref="U1:X1"/>
     <mergeCell ref="Y8:AB8"/>
+    <mergeCell ref="Y9:AB9"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="AC1:AF2"/>
+    <mergeCell ref="AC3:AF3"/>
+    <mergeCell ref="AC4:AF4"/>
+    <mergeCell ref="AC5:AF5"/>
+    <mergeCell ref="AC11:AF11"/>
+    <mergeCell ref="AC6:AF6"/>
+    <mergeCell ref="AC7:AF7"/>
+    <mergeCell ref="AC8:AF8"/>
+    <mergeCell ref="AC9:AF9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -10054,6 +10457,29 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <SharedWithUsers xmlns="c5ae091c-4d86-42b7-bd6d-05a6d5850206">
+      <UserInfo>
+        <DisplayName>Integrantes de la CURSO 1º MUSE</DisplayName>
+        <AccountId>16</AccountId>
+        <AccountType/>
+      </UserInfo>
+    </SharedWithUsers>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001E172B7A065CA14588F69A7125C5BD0C" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="c347a13695a8e345f3a646912ba294d8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e396dde7-6e29-4e2b-9948-8bd66cb2bb47" xmlns:ns3="c5ae091c-4d86-42b7-bd6d-05a6d5850206" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c01a5560f28fea09b4ea7e239530bc69" ns2:_="" ns3:_="">
     <xsd:import namespace="e396dde7-6e29-4e2b-9948-8bd66cb2bb47"/>
@@ -10218,30 +10644,25 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <SharedWithUsers xmlns="c5ae091c-4d86-42b7-bd6d-05a6d5850206">
-      <UserInfo>
-        <DisplayName>Integrantes de la CURSO 1º MUSE</DisplayName>
-        <AccountId>16</AccountId>
-        <AccountType/>
-      </UserInfo>
-    </SharedWithUsers>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A54CB81-BDC2-4F30-B8AA-8FF202FE488F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F2DDC3-8EF2-4F40-AEC5-CBD2E661EA55}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c5ae091c-4d86-42b7-bd6d-05a6d5850206"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{427DAEE4-79A2-4E1E-ADBA-A982983815DD}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10258,22 +10679,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{76F2DDC3-8EF2-4F40-AEC5-CBD2E661EA55}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c5ae091c-4d86-42b7-bd6d-05a6d5850206"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A54CB81-BDC2-4F30-B8AA-8FF202FE488F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
why was this not uploaded b4
</commit_message>
<xml_diff>
--- a/MicroSat/Iteraciones.xlsx
+++ b/MicroSat/Iteraciones.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\diego\Documents\MEng Space Systems (Local)\2. EUE\Micro-Satellite Design &amp; Analysis\MicroSat\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1454E8EE-DCB6-4CF9-93C8-EEFC952E4A60}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{361AC6B6-3D36-4379-8B63-4FFCFF2C46E9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-105" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8850" yWindow="5190" windowWidth="17280" windowHeight="8970" tabRatio="867" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="It_Bandeja Inf" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="923" uniqueCount="123">
   <si>
     <t>Nº rigidizadores</t>
   </si>
@@ -405,6 +405,9 @@
   </si>
   <si>
     <t>sat_bandeja_inf_9rig_i_al7075_OPTIMIZACION_SOL6 (MISMA LONG RIG)</t>
+  </si>
+  <si>
+    <t>Ti</t>
   </si>
 </sst>
 </file>
@@ -2272,7 +2275,7 @@
   <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="P12" sqref="P12"/>
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3837,23 +3840,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8673FD-1E69-4B06-A1F3-8979D136D77F}">
-  <dimension ref="A2:L23"/>
+  <dimension ref="A2:P56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="4.44140625" customWidth="1"/>
-    <col min="4" max="4" width="4.33203125" customWidth="1"/>
-    <col min="5" max="5" width="4.109375" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" customWidth="1"/>
-    <col min="7" max="7" width="5.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" customWidth="1"/>
-    <col min="9" max="9" width="8.109375" customWidth="1"/>
+    <col min="1" max="1" width="9.5546875" customWidth="1"/>
+    <col min="2" max="2" width="9" customWidth="1"/>
+    <col min="3" max="3" width="4.44140625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="4.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="4.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="5.109375" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" hidden="1" customWidth="1"/>
     <col min="10" max="10" width="1.5546875" customWidth="1"/>
     <col min="15" max="15" width="17.88671875" customWidth="1"/>
   </cols>
@@ -4206,7 +4209,7 @@
         <v>45.988584537991642</v>
       </c>
     </row>
-    <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="183">
         <v>965000</v>
       </c>
@@ -4244,7 +4247,7 @@
         <v>290.1831456343939</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A20" s="190" t="s">
         <v>105</v>
       </c>
@@ -4256,7 +4259,7 @@
       <c r="G20" s="189"/>
       <c r="H20" s="189"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A21" s="189" t="s">
         <v>106</v>
       </c>
@@ -4274,7 +4277,7 @@
         <v>271000000</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A22" s="189"/>
       <c r="B22" s="189"/>
       <c r="C22" s="189"/>
@@ -4284,7 +4287,7 @@
       <c r="G22" s="189"/>
       <c r="H22" s="189"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A23" s="189" t="s">
         <v>108</v>
       </c>
@@ -4302,11 +4305,795 @@
         <v>280000000</v>
       </c>
     </row>
+    <row r="25" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A26" s="212" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="213"/>
+      <c r="C26" s="213"/>
+      <c r="D26" s="213"/>
+      <c r="E26" s="213"/>
+      <c r="F26" s="213"/>
+      <c r="G26" s="213"/>
+      <c r="H26" s="213"/>
+      <c r="I26" s="213"/>
+      <c r="J26" s="213"/>
+      <c r="K26" s="213"/>
+      <c r="L26" s="214"/>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A27" s="182" t="s">
+        <v>89</v>
+      </c>
+      <c r="B27" s="186"/>
+      <c r="C27" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D27" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F27" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G27" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H27" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I27" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J27" s="178"/>
+      <c r="K27" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L27" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="183">
+        <v>39100000</v>
+      </c>
+      <c r="B28" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C28" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D28" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E28" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F28" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G28" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H28" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I28" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J28" s="180"/>
+      <c r="K28" s="184">
+        <f>(H28/(A28*C28*D28*E28*F28))-1</f>
+        <v>5.9495017815704321</v>
+      </c>
+      <c r="L28" s="185">
+        <f>(I28/(A28*C28*D28*E28*G28))-1</f>
+        <v>6.1864893999281332</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="183">
+        <v>23100000</v>
+      </c>
+      <c r="B29" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C29" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D29" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E29" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F29" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G29" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H29" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I29" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J29" s="180"/>
+      <c r="K29" s="184">
+        <f>(H29/(A29*C29*D29*E29*F29))-1</f>
+        <v>10.763009509065101</v>
+      </c>
+      <c r="L29" s="185">
+        <f>(I29/(A29*C29*D29*E29*G29))-1</f>
+        <v>11.164144395549352</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="O30" s="181">
+        <v>880000000</v>
+      </c>
+      <c r="P30" s="181">
+        <v>950000000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A31" s="212" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="213"/>
+      <c r="C31" s="213"/>
+      <c r="D31" s="213"/>
+      <c r="E31" s="213"/>
+      <c r="F31" s="213"/>
+      <c r="G31" s="213"/>
+      <c r="H31" s="213"/>
+      <c r="I31" s="213"/>
+      <c r="J31" s="213"/>
+      <c r="K31" s="213"/>
+      <c r="L31" s="214"/>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A32" s="182" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="186"/>
+      <c r="C32" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E32" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G32" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H32" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I32" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J32" s="178"/>
+      <c r="K32" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L32" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="183">
+        <v>75300000</v>
+      </c>
+      <c r="B33" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C33" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D33" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E33" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F33" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G33" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H33" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I33" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J33" s="180"/>
+      <c r="K33" s="184">
+        <f>(H33/(A33*C33*D33*E33*F33))-1</f>
+        <v>2.6085726382390955</v>
+      </c>
+      <c r="L33" s="184">
+        <f>(I33/(A33*C33*D33*E33*G33))-1</f>
+        <v>2.7316299540131479</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="183">
+        <v>46300000</v>
+      </c>
+      <c r="B34" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D34" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E34" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F34" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G34" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H34" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I34" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J34" s="180"/>
+      <c r="K34" s="184">
+        <f>(H34/(A34*C34*D34*E34*F34))-1</f>
+        <v>4.8688017205054823</v>
+      </c>
+      <c r="L34" s="184">
+        <f>(I34/(A34*C34*D34*E34*G34))-1</f>
+        <v>5.0689359727254866</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="155"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A36" s="212" t="s">
+        <v>101</v>
+      </c>
+      <c r="B36" s="213"/>
+      <c r="C36" s="213"/>
+      <c r="D36" s="213"/>
+      <c r="E36" s="213"/>
+      <c r="F36" s="213"/>
+      <c r="G36" s="213"/>
+      <c r="H36" s="213"/>
+      <c r="I36" s="213"/>
+      <c r="J36" s="213"/>
+      <c r="K36" s="213"/>
+      <c r="L36" s="214"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A37" s="182" t="s">
+        <v>99</v>
+      </c>
+      <c r="B37" s="186"/>
+      <c r="C37" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D37" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E37" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F37" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H37" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J37" s="178"/>
+      <c r="K37" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L37" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="183">
+        <v>75300000</v>
+      </c>
+      <c r="B38" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C38" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D38" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E38" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F38" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G38" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H38" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I38" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J38" s="180"/>
+      <c r="K38" s="184">
+        <f>(H38/(A38*C38*D38*E38*F38))-1</f>
+        <v>2.6085726382390955</v>
+      </c>
+      <c r="L38" s="185">
+        <f>(I38/(A38*C38*D38*E38*G38))-1</f>
+        <v>2.7316299540131479</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="183">
+        <v>46600000</v>
+      </c>
+      <c r="B39" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D39" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E39" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F39" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G39" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H39" s="181">
+        <v>434000000</v>
+      </c>
+      <c r="I39" s="181">
+        <v>510000000</v>
+      </c>
+      <c r="J39" s="180"/>
+      <c r="K39" s="184">
+        <f>(H39/(A39*C39*D39*E39*F39))-1</f>
+        <v>4.8310197351803401</v>
+      </c>
+      <c r="L39" s="185">
+        <f>(I39/(A39*C39*D39*E39*G39))-1</f>
+        <v>5.0298655694675976</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A43" s="212" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="213"/>
+      <c r="C43" s="213"/>
+      <c r="D43" s="213"/>
+      <c r="E43" s="213"/>
+      <c r="F43" s="213"/>
+      <c r="G43" s="213"/>
+      <c r="H43" s="213"/>
+      <c r="I43" s="213"/>
+      <c r="J43" s="213"/>
+      <c r="K43" s="213"/>
+      <c r="L43" s="214"/>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A44" s="182" t="s">
+        <v>89</v>
+      </c>
+      <c r="B44" s="186"/>
+      <c r="C44" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D44" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E44" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G44" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H44" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I44" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J44" s="178"/>
+      <c r="K44" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L44" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="183">
+        <v>133000000</v>
+      </c>
+      <c r="B45" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C45" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D45" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E45" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F45" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G45" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H45" s="181">
+        <v>880000000</v>
+      </c>
+      <c r="I45" s="181">
+        <v>950000000</v>
+      </c>
+      <c r="J45" s="180"/>
+      <c r="K45" s="184">
+        <f>(H45/(A45*C45*D45*E45*F45))-1</f>
+        <v>3.1425878746452893</v>
+      </c>
+      <c r="L45" s="185">
+        <f>(I45/(A45*C45*D45*E45*G45))-1</f>
+        <v>2.935458480913026</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="183">
+        <v>51300000</v>
+      </c>
+      <c r="B46" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C46" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D46" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E46" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F46" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G46" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H46" s="181">
+        <v>880000000</v>
+      </c>
+      <c r="I46" s="181">
+        <v>950000000</v>
+      </c>
+      <c r="J46" s="180"/>
+      <c r="K46" s="184">
+        <f>(H46/(A46*C46*D46*E46*F46))-1</f>
+        <v>9.7400426379692728</v>
+      </c>
+      <c r="L46" s="185">
+        <f>(I46/(A46*C46*D46*E46*G46))-1</f>
+        <v>9.2030405060708098</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A48" s="212" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="213"/>
+      <c r="C48" s="213"/>
+      <c r="D48" s="213"/>
+      <c r="E48" s="213"/>
+      <c r="F48" s="213"/>
+      <c r="G48" s="213"/>
+      <c r="H48" s="213"/>
+      <c r="I48" s="213"/>
+      <c r="J48" s="213"/>
+      <c r="K48" s="213"/>
+      <c r="L48" s="214"/>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A49" s="182" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="186"/>
+      <c r="C49" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D49" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E49" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F49" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G49" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H49" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I49" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J49" s="178"/>
+      <c r="K49" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L49" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="183">
+        <v>222000000</v>
+      </c>
+      <c r="B50" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D50" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E50" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F50" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G50" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H50" s="181">
+        <v>880000000</v>
+      </c>
+      <c r="I50" s="181">
+        <v>950000000</v>
+      </c>
+      <c r="J50" s="180"/>
+      <c r="K50" s="184">
+        <f>(H50/(A50*C50*D50*E50*F50))-1</f>
+        <v>1.4818206636388456</v>
+      </c>
+      <c r="L50" s="184">
+        <f>(I50/(A50*C50*D50*E50*G50))-1</f>
+        <v>1.3577296304569031</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="183">
+        <v>115000000</v>
+      </c>
+      <c r="B51" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C51" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D51" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E51" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F51" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G51" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H51" s="181">
+        <v>880000000</v>
+      </c>
+      <c r="I51" s="181">
+        <v>950000000</v>
+      </c>
+      <c r="J51" s="180"/>
+      <c r="K51" s="184">
+        <f>(H51/(A51*C51*D51*E51*F51))-1</f>
+        <v>3.7909929332854233</v>
+      </c>
+      <c r="L51" s="184">
+        <f>(I51/(A51*C51*D51*E51*G51))-1</f>
+        <v>3.5514432866211525</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="155"/>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A53" s="212" t="s">
+        <v>101</v>
+      </c>
+      <c r="B53" s="213"/>
+      <c r="C53" s="213"/>
+      <c r="D53" s="213"/>
+      <c r="E53" s="213"/>
+      <c r="F53" s="213"/>
+      <c r="G53" s="213"/>
+      <c r="H53" s="213"/>
+      <c r="I53" s="213"/>
+      <c r="J53" s="213"/>
+      <c r="K53" s="213"/>
+      <c r="L53" s="214"/>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A54" s="182" t="s">
+        <v>99</v>
+      </c>
+      <c r="B54" s="186"/>
+      <c r="C54" s="178" t="s">
+        <v>90</v>
+      </c>
+      <c r="D54" s="178" t="s">
+        <v>91</v>
+      </c>
+      <c r="E54" s="178" t="s">
+        <v>92</v>
+      </c>
+      <c r="F54" s="178" t="s">
+        <v>93</v>
+      </c>
+      <c r="G54" s="178" t="s">
+        <v>94</v>
+      </c>
+      <c r="H54" s="178" t="s">
+        <v>95</v>
+      </c>
+      <c r="I54" s="178" t="s">
+        <v>96</v>
+      </c>
+      <c r="J54" s="178"/>
+      <c r="K54" s="178" t="s">
+        <v>97</v>
+      </c>
+      <c r="L54" s="179" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="183">
+        <v>222000000</v>
+      </c>
+      <c r="B55" s="187" t="s">
+        <v>102</v>
+      </c>
+      <c r="C55" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D55" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E55" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F55" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G55" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H55" s="181">
+        <v>880000000</v>
+      </c>
+      <c r="I55" s="181">
+        <v>950000000</v>
+      </c>
+      <c r="J55" s="180"/>
+      <c r="K55" s="184">
+        <f>(H55/(A55*C55*D55*E55*F55))-1</f>
+        <v>1.4818206636388456</v>
+      </c>
+      <c r="L55" s="185">
+        <f>(I55/(A55*C55*D55*E55*G55))-1</f>
+        <v>1.3577296304569031</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="183">
+        <v>44800000</v>
+      </c>
+      <c r="B56" s="187" t="s">
+        <v>103</v>
+      </c>
+      <c r="C56" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D56" s="180">
+        <v>1.2</v>
+      </c>
+      <c r="E56" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F56" s="180">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="G56" s="180">
+        <v>1.25</v>
+      </c>
+      <c r="H56" s="181">
+        <v>880000000</v>
+      </c>
+      <c r="I56" s="181">
+        <v>950000000</v>
+      </c>
+      <c r="J56" s="180"/>
+      <c r="K56" s="184">
+        <f>(H56/(A56*C56*D56*E56*F56))-1</f>
+        <v>11.298307752853205</v>
+      </c>
+      <c r="L56" s="185">
+        <f>(I56/(A56*C56*D56*E56*G56))-1</f>
+        <v>10.683392365210544</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="9">
+    <mergeCell ref="A43:L43"/>
+    <mergeCell ref="A48:L48"/>
+    <mergeCell ref="A53:L53"/>
+    <mergeCell ref="A36:L36"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="A14:L14"/>
+    <mergeCell ref="A26:L26"/>
+    <mergeCell ref="A31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4317,8 +5104,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA3D57E-AF43-4403-B1EC-4764DD27CECF}">
   <dimension ref="A2:L104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A105" sqref="A105"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6722,6 +7509,8 @@
     <mergeCell ref="A83:L83"/>
     <mergeCell ref="A78:L78"/>
     <mergeCell ref="A73:L73"/>
+    <mergeCell ref="A4:L4"/>
+    <mergeCell ref="A9:L9"/>
     <mergeCell ref="A38:L38"/>
     <mergeCell ref="A43:L43"/>
     <mergeCell ref="A48:L48"/>
@@ -6729,8 +7518,6 @@
     <mergeCell ref="A21:L21"/>
     <mergeCell ref="A26:L26"/>
     <mergeCell ref="A31:L31"/>
-    <mergeCell ref="A4:L4"/>
-    <mergeCell ref="A9:L9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6740,8 +7527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A7277F0-43A1-4A40-97D9-A023F961F6A8}">
   <dimension ref="A2:L68"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="M69" sqref="A54:M69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7613,7 +8400,7 @@
     </row>
     <row r="40" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="183">
-        <v>85600000</v>
+        <v>66500000</v>
       </c>
       <c r="B40" s="187" t="s">
         <v>102</v>
@@ -7642,16 +8429,16 @@
       <c r="J40" s="180"/>
       <c r="K40" s="184">
         <f>(H40/(A40*C40*D40*E40*F40))-1</f>
-        <v>2.1743635474229426</v>
+        <v>3.086098039991036</v>
       </c>
       <c r="L40" s="185">
         <f>(I40/(A40*C40*D40*E40*G40))-1</f>
-        <v>2.2826137329110985</v>
+        <v>3.2254396321381966</v>
       </c>
     </row>
     <row r="41" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="183">
-        <v>43000000</v>
+        <v>38100000</v>
       </c>
       <c r="B41" s="187" t="s">
         <v>103</v>
@@ -7680,11 +8467,11 @@
       <c r="J41" s="180"/>
       <c r="K41" s="184">
         <f>(H41/(A41*C41*D41*E41*F41))-1</f>
-        <v>5.3191981316140442</v>
+        <v>6.1319034031339603</v>
       </c>
       <c r="L41" s="185">
         <f>(I41/(A41*C41*D41*E41*G41))-1</f>
-        <v>5.5346915241206984</v>
+        <v>6.3751111689551188</v>
       </c>
     </row>
     <row r="42" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -7740,7 +8527,7 @@
     </row>
     <row r="45" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="183">
-        <v>83500000</v>
+        <v>74600000</v>
       </c>
       <c r="B45" s="187" t="s">
         <v>102</v>
@@ -7769,16 +8556,16 @@
       <c r="J45" s="180"/>
       <c r="K45" s="184">
         <f>(H45/(A45*C45*D45*E45*F45))-1</f>
-        <v>2.2541978402323819</v>
+        <v>2.6424332394021968</v>
       </c>
       <c r="L45" s="184">
         <f>(I45/(A45*C45*D45*E45*G45))-1</f>
-        <v>2.3651704854753297</v>
+        <v>2.7666452484878019</v>
       </c>
     </row>
     <row r="46" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="183">
-        <v>64400000</v>
+        <v>42500000</v>
       </c>
       <c r="B46" s="187" t="s">
         <v>103</v>
@@ -7807,11 +8594,11 @@
       <c r="J46" s="180"/>
       <c r="K46" s="184">
         <f>(H46/(A46*C46*D46*E46*F46))-1</f>
-        <v>3.2193403673820482</v>
+        <v>5.3935416390447974</v>
       </c>
       <c r="L46" s="184">
         <f>(I46/(A46*C46*D46*E46*G46))-1</f>
-        <v>3.3632257070992244</v>
+        <v>5.6115702479338827</v>
       </c>
     </row>
     <row r="47" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -7867,7 +8654,7 @@
     </row>
     <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="183">
-        <v>83500000</v>
+        <v>74600000</v>
       </c>
       <c r="B50" s="187" t="s">
         <v>102</v>
@@ -7896,16 +8683,16 @@
       <c r="J50" s="180"/>
       <c r="K50" s="184">
         <f>(H50/(A50*C50*D50*E50*F50))-1</f>
-        <v>2.2541978402323819</v>
+        <v>2.6424332394021968</v>
       </c>
       <c r="L50" s="185">
         <f>(I50/(A50*C50*D50*E50*G50))-1</f>
-        <v>2.3651704854753297</v>
+        <v>2.7666452484878019</v>
       </c>
     </row>
     <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="183">
-        <v>44200000</v>
+        <v>43000000</v>
       </c>
       <c r="B51" s="187" t="s">
         <v>103</v>
@@ -7934,11 +8721,11 @@
       <c r="J51" s="180"/>
       <c r="K51" s="184">
         <f>(H51/(A51*C51*D51*E51*F51))-1</f>
-        <v>5.1476361913892283</v>
+        <v>5.3191981316140442</v>
       </c>
       <c r="L51" s="185">
         <f>(I51/(A51*C51*D51*E51*G51))-1</f>
-        <v>5.357279084551811</v>
+        <v>5.5346915241206984</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.3">
@@ -8010,7 +8797,7 @@
     </row>
     <row r="57" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="183">
-        <v>72400000</v>
+        <v>55700000</v>
       </c>
       <c r="B57" s="187" t="s">
         <v>102</v>
@@ -8039,16 +8826,16 @@
       <c r="J57" s="180"/>
       <c r="K57" s="184">
         <f>(H57/(A57*C57*D57*E57*F57))-1</f>
-        <v>2.7531149124227055</v>
+        <v>3.8783755773681143</v>
       </c>
       <c r="L57" s="185">
         <f>(I57/(A57*C57*D57*E57*G57))-1</f>
-        <v>2.8811013195744484</v>
+        <v>4.0447349288543997</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A58" s="183">
-        <v>40800000</v>
+        <v>33000000</v>
       </c>
       <c r="B58" s="187" t="s">
         <v>103</v>
@@ -8077,11 +8864,11 @@
       <c r="J58" s="180"/>
       <c r="K58" s="184">
         <f>(H58/(A58*C58*D58*E58*F58))-1</f>
-        <v>5.659939207338331</v>
+        <v>7.2341066563455723</v>
       </c>
       <c r="L58" s="185">
         <f>(I58/(A58*C58*D58*E58*G58))-1</f>
-        <v>5.8870523415977951</v>
+        <v>7.5149010768845468</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -8137,7 +8924,7 @@
     </row>
     <row r="62" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A62" s="183">
-        <v>84400000</v>
+        <v>74300000</v>
       </c>
       <c r="B62" s="187" t="s">
         <v>102</v>
@@ -8166,16 +8953,16 @@
       <c r="J62" s="180"/>
       <c r="K62" s="184">
         <f>(H62/(A62*C62*D62*E62*F62))-1</f>
-        <v>2.219496678428956</v>
+        <v>2.6571402376770377</v>
       </c>
       <c r="L62" s="184">
         <f>(I62/(A62*C62*D62*E62*G62))-1</f>
-        <v>2.3292859660804504</v>
+        <v>2.7818537757360704</v>
       </c>
     </row>
     <row r="63" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="183">
-        <v>65600000</v>
+        <v>43900000</v>
       </c>
       <c r="B63" s="187" t="s">
         <v>103</v>
@@ -8204,11 +8991,11 @@
       <c r="J63" s="180"/>
       <c r="K63" s="184">
         <f>(H63/(A63*C63*D63*E63*F63))-1</f>
-        <v>3.1421573118811565</v>
+        <v>5.1896473726515691</v>
       </c>
       <c r="L63" s="184">
         <f>(I63/(A63*C63*D63*E63*G63))-1</f>
-        <v>3.2834106027010677</v>
+        <v>5.4007229051751713</v>
       </c>
     </row>
     <row r="64" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -8264,7 +9051,7 @@
     </row>
     <row r="67" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="183">
-        <v>84400000</v>
+        <v>74300000</v>
       </c>
       <c r="B67" s="187" t="s">
         <v>102</v>
@@ -8293,16 +9080,16 @@
       <c r="J67" s="180"/>
       <c r="K67" s="184">
         <f>(H67/(A67*C67*D67*E67*F67))-1</f>
-        <v>2.219496678428956</v>
+        <v>2.6571402376770377</v>
       </c>
       <c r="L67" s="185">
         <f>(I67/(A67*C67*D67*E67*G67))-1</f>
-        <v>2.3292859660804504</v>
+        <v>2.7818537757360704</v>
       </c>
     </row>
     <row r="68" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A68" s="183">
-        <v>46200000</v>
+        <v>44700000</v>
       </c>
       <c r="B68" s="187" t="s">
         <v>103</v>
@@ -8331,11 +9118,11 @@
       <c r="J68" s="180"/>
       <c r="K68" s="184">
         <f>(H68/(A68*C68*D68*E68*F68))-1</f>
-        <v>4.8815047545325507</v>
+        <v>5.0788706858927046</v>
       </c>
       <c r="L68" s="185">
         <f>(I68/(A68*C68*D68*E68*G68))-1</f>
-        <v>5.0820721977746759</v>
+        <v>5.2861685802503366</v>
       </c>
     </row>
   </sheetData>
@@ -8346,12 +9133,12 @@
     <mergeCell ref="A38:L38"/>
     <mergeCell ref="A43:L43"/>
     <mergeCell ref="A48:L48"/>
+    <mergeCell ref="A31:L31"/>
     <mergeCell ref="A4:L4"/>
     <mergeCell ref="A9:L9"/>
     <mergeCell ref="A14:L14"/>
     <mergeCell ref="A21:L21"/>
     <mergeCell ref="A26:L26"/>
-    <mergeCell ref="A31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8361,8 +9148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C65A9CD-A62A-4089-A8C2-03B1AF135CF1}">
   <dimension ref="A2:L53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O40" sqref="O40"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H24" sqref="H24:I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8461,19 +9248,19 @@
         <v>1.25</v>
       </c>
       <c r="H6" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I6" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J6" s="180"/>
       <c r="K6" s="184">
         <f>(H6/(A6*C6*D6*E6*F6))-1</f>
-        <v>1.3224403389692641</v>
+        <v>3.7090956181865264</v>
       </c>
       <c r="L6" s="185">
         <f>(I6/(A6*C6*D6*E6*G6))-1</f>
-        <v>1.4016387652751288</v>
+        <v>3.473640837277201</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8499,19 +9286,19 @@
         <v>1.25</v>
       </c>
       <c r="H7" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I7" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J7" s="180"/>
       <c r="K7" s="184">
         <f>(H7/(A7*C7*D7*E7*F7))-1</f>
-        <v>5.3191981316140442</v>
+        <v>11.813120635530781</v>
       </c>
       <c r="L7" s="185">
         <f>(I7/(A7*C7*D7*E7*G7))-1</f>
-        <v>5.5346915241206984</v>
+        <v>11.172464603754243</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -8588,19 +9375,19 @@
         <v>1.25</v>
       </c>
       <c r="H11" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I11" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J11" s="180"/>
       <c r="K11" s="184">
         <f>(H11/(A11*C11*D11*E11*F11))-1</f>
-        <v>1.043049019995518</v>
+        <v>3.1425878746452893</v>
       </c>
       <c r="L11" s="184">
         <f>(I11/(A11*C11*D11*E11*G11))-1</f>
-        <v>1.1127198160690983</v>
+        <v>2.935458480913026</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8626,19 +9413,19 @@
         <v>1.25</v>
       </c>
       <c r="H12" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I12" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J12" s="180"/>
       <c r="K12" s="184">
         <f>(H12/(A12*C12*D12*E12*F12))-1</f>
-        <v>1.7670623183238683</v>
+        <v>4.6106332721774281</v>
       </c>
       <c r="L12" s="184">
         <f>(I12/(A12*C12*D12*E12*G12))-1</f>
-        <v>1.8614229688104893</v>
+        <v>4.3301016085685582</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -8715,19 +9502,19 @@
         <v>1.25</v>
       </c>
       <c r="H16" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I16" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J16" s="180"/>
       <c r="K16" s="184">
         <f>(H16/(A16*C16*D16*E16*F16))-1</f>
-        <v>1.043049019995518</v>
+        <v>3.1425878746452893</v>
       </c>
       <c r="L16" s="185">
         <f>(I16/(A16*C16*D16*E16*G16))-1</f>
-        <v>1.1127198160690983</v>
+        <v>2.935458480913026</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8753,19 +9540,19 @@
         <v>1.25</v>
       </c>
       <c r="H17" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I17" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J17" s="180"/>
       <c r="K17" s="184">
         <f>(H17/(A17*C17*D17*E17*F17))-1</f>
-        <v>3.2457112446781853</v>
+        <v>7.6088154269972428</v>
       </c>
       <c r="L17" s="185">
         <f>(I17/(A17*C17*D17*E17*G17))-1</f>
-        <v>3.3904958677685944</v>
+        <v>7.1783746556473815</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -8858,19 +9645,19 @@
         <v>1.25</v>
       </c>
       <c r="H24" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I24" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J24" s="180"/>
       <c r="K24" s="184">
         <f>(H24/(A24*C24*D24*E24*F24))-1</f>
-        <v>1.4046506164549024</v>
+        <v>3.8757892683878206</v>
       </c>
       <c r="L24" s="185">
         <f>(I24/(A24*C24*D24*E24*G24))-1</f>
-        <v>1.4866525268777884</v>
+        <v>3.6319998049684292</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -8896,19 +9683,19 @@
         <v>1.25</v>
       </c>
       <c r="H25" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I25" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J25" s="180"/>
       <c r="K25" s="184">
         <f>(H25/(A25*C25*D25*E25*F25))-1</f>
-        <v>5.6763026943342476</v>
+        <v>12.537203619848245</v>
       </c>
       <c r="L25" s="185">
         <f>(I25/(A25*C25*D25*E25*G25))-1</f>
-        <v>5.9039738461226055</v>
+        <v>11.860343438855834</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -8985,19 +9772,19 @@
         <v>1.25</v>
       </c>
       <c r="H29" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I29" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J29" s="180"/>
       <c r="K29" s="184">
         <f>(H29/(A29*C29*D29*E29*F29))-1</f>
-        <v>1.2272583578639664</v>
+        <v>3.5160998961297016</v>
       </c>
       <c r="L29" s="184">
         <f>(I29/(A29*C29*D29*E29*G29))-1</f>
-        <v>1.3032109470261481</v>
+        <v>3.2902949013232172</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9023,19 +9810,19 @@
         <v>1.25</v>
       </c>
       <c r="H30" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I30" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J30" s="180"/>
       <c r="K30" s="184">
         <f>(H30/(A30*C30*D30*E30*F30))-1</f>
-        <v>2.0225308082247375</v>
+        <v>5.1286338968612188</v>
       </c>
       <c r="L30" s="184">
         <f>(I30/(A30*C30*D30*E30*G30))-1</f>
-        <v>2.1256032873992217</v>
+        <v>4.8222022020181576</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -9112,19 +9899,19 @@
         <v>1.25</v>
       </c>
       <c r="H34" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I34" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J34" s="180"/>
       <c r="K34" s="184">
         <f>(H34/(A34*C34*D34*E34*F34))-1</f>
-        <v>1.2272583578639664</v>
+        <v>3.5160998961297016</v>
       </c>
       <c r="L34" s="185">
         <f>(I34/(A34*C34*D34*E34*G34))-1</f>
-        <v>1.3032109470261481</v>
+        <v>3.2902949013232172</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9150,19 +9937,19 @@
         <v>1.25</v>
       </c>
       <c r="H35" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I35" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J35" s="180"/>
       <c r="K35" s="184">
         <f>(H35/(A35*C35*D35*E35*F35))-1</f>
-        <v>3.6768592023993785</v>
+        <v>8.4830324841277722</v>
       </c>
       <c r="L35" s="185">
         <f>(I35/(A35*C35*D35*E35*G35))-1</f>
-        <v>3.8363465669051653</v>
+        <v>8.0088808599213852</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.3">
@@ -9255,19 +10042,19 @@
         <v>1.25</v>
       </c>
       <c r="H42" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I42" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J42" s="180"/>
       <c r="K42" s="184">
         <f>(H42/(A42*C42*D42*E42*F42))-1</f>
-        <v>1.3628306057339477</v>
+        <v>3.7909929332854233</v>
       </c>
       <c r="L42" s="185">
         <f>(I42/(A42*C42*D42*E42*G42))-1</f>
-        <v>1.4434063959755661</v>
+        <v>3.5514432866211525</v>
       </c>
     </row>
     <row r="43" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9293,19 +10080,19 @@
         <v>1.25</v>
       </c>
       <c r="H43" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I43" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J43" s="180"/>
       <c r="K43" s="184">
         <f>(H43/(A43*C43*D43*E43*F43))-1</f>
-        <v>5.5318634533510549</v>
+        <v>12.244331426149605</v>
       </c>
       <c r="L43" s="185">
         <f>(I43/(A43*C43*D43*E43*G43))-1</f>
-        <v>5.7546090273362989</v>
+        <v>11.582114854842125</v>
       </c>
     </row>
     <row r="44" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -9382,19 +10169,19 @@
         <v>1.25</v>
       </c>
       <c r="H47" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I47" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J47" s="180"/>
       <c r="K47" s="184">
         <f>(H47/(A47*C47*D47*E47*F47))-1</f>
-        <v>1.1395710209401884</v>
+        <v>3.3383006876206585</v>
       </c>
       <c r="L47" s="184">
         <f>(I47/(A47*C47*D47*E47*G47))-1</f>
-        <v>1.2125333506865359</v>
+        <v>3.121385653239626</v>
       </c>
     </row>
     <row r="48" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9420,19 +10207,19 @@
         <v>1.25</v>
       </c>
       <c r="H48" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I48" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J48" s="180"/>
       <c r="K48" s="184">
         <f>(H48/(A48*C48*D48*E48*F48))-1</f>
-        <v>1.8906970176532325</v>
+        <v>4.8613211417853561</v>
       </c>
       <c r="L48" s="184">
         <f>(I48/(A48*C48*D48*E48*G48))-1</f>
-        <v>1.9892737823105322</v>
+        <v>4.5682550846960899</v>
       </c>
     </row>
     <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
@@ -9509,19 +10296,19 @@
         <v>1.25</v>
       </c>
       <c r="H52" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I52" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J52" s="180"/>
       <c r="K52" s="184">
         <f>(H52/(A52*C52*D52*E52*F52))-1</f>
-        <v>1.1395710209401884</v>
+        <v>3.3383006876206585</v>
       </c>
       <c r="L52" s="185">
         <f>(I52/(A52*C52*D52*E52*G52))-1</f>
-        <v>1.2125333506865359</v>
+        <v>3.121385653239626</v>
       </c>
     </row>
     <row r="53" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9547,19 +10334,19 @@
         <v>1.25</v>
       </c>
       <c r="H53" s="181">
-        <v>434000000</v>
+        <v>880000000</v>
       </c>
       <c r="I53" s="181">
-        <v>510000000</v>
+        <v>950000000</v>
       </c>
       <c r="J53" s="180"/>
       <c r="K53" s="184">
         <f>(H53/(A53*C53*D53*E53*F53))-1</f>
-        <v>3.4618311930936603</v>
+        <v>8.0470309906046573</v>
       </c>
       <c r="L53" s="185">
         <f>(I53/(A53*C53*D53*E53*G53))-1</f>
-        <v>3.613985805208376</v>
+        <v>7.5946794410744261</v>
       </c>
     </row>
   </sheetData>
@@ -9583,7 +10370,7 @@
   <dimension ref="A1:AF28"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>